<commit_message>
added FM to the dataset_harmonization
</commit_message>
<xml_diff>
--- a/interlab_comparison/harmonized_dataset.xlsx
+++ b/interlab_comparison/harmonized_dataset.xlsx
@@ -7609,7 +7609,7 @@
         <v>2.616199533674754</v>
       </c>
       <c r="E312" t="n">
-        <v>0.9535404943665061</v>
+        <v>1.186388313787428</v>
       </c>
       <c r="F312" t="n">
         <v>0.00261</v>
@@ -7632,7 +7632,7 @@
         <v>2.636152499382386</v>
       </c>
       <c r="E313" t="n">
-        <v>0.9552109418258912</v>
+        <v>1.188212007838675</v>
       </c>
       <c r="F313" t="n">
         <v>0.00263</v>
@@ -7678,7 +7678,7 @@
         <v>3.554560451026259</v>
       </c>
       <c r="E315" t="n">
-        <v>0.9505243521961335</v>
+        <v>1.183114511951071</v>
       </c>
       <c r="F315" t="n">
         <v>0.00355</v>
@@ -7701,7 +7701,7 @@
         <v>4.083968658057993</v>
       </c>
       <c r="E316" t="n">
-        <v>0.9495471225511716</v>
+        <v>1.182055195234465</v>
       </c>
       <c r="F316" t="n">
         <v>0.00408</v>
@@ -7724,7 +7724,7 @@
         <v>2.067849124090053</v>
       </c>
       <c r="E317" t="n">
-        <v>0.9536050845606593</v>
+        <v>1.186480649503066</v>
       </c>
       <c r="F317" t="n">
         <v>0.00206</v>
@@ -7770,7 +7770,7 @@
         <v>4.543566880766695</v>
       </c>
       <c r="E319" t="n">
-        <v>0.9416917389332611</v>
+        <v>1.173497409834919</v>
       </c>
       <c r="F319" t="n">
         <v>0.00454</v>
@@ -7793,7 +7793,7 @@
         <v>2.616199533674754</v>
       </c>
       <c r="E320" t="n">
-        <v>0.9568543711789497</v>
+        <v>1.190027668053222</v>
       </c>
       <c r="F320" t="n">
         <v>0.00261</v>
@@ -7816,7 +7816,7 @@
         <v>2.616199533674754</v>
       </c>
       <c r="E321" t="n">
-        <v>0.9522673541880522</v>
+        <v>1.185040562992661</v>
       </c>
       <c r="F321" t="n">
         <v>0.00261</v>
@@ -7839,7 +7839,7 @@
         <v>3.005395148728367</v>
       </c>
       <c r="E322" t="n">
-        <v>0.9498052358467118</v>
+        <v>1.182364089244737</v>
       </c>
       <c r="F322" t="n">
         <v>0.003</v>
@@ -7885,7 +7885,7 @@
         <v>3.005395148728367</v>
       </c>
       <c r="E324" t="n">
-        <v>0.9479619290959594</v>
+        <v>1.180360450866756</v>
       </c>
       <c r="F324" t="n">
         <v>0.003</v>
@@ -7908,7 +7908,7 @@
         <v>3.005395148728367</v>
       </c>
       <c r="E325" t="n">
-        <v>0.9516493790962209</v>
+        <v>1.184383998095519</v>
       </c>
       <c r="F325" t="n">
         <v>0.003</v>
@@ -7931,7 +7931,7 @@
         <v>3.005395148728367</v>
       </c>
       <c r="E326" t="n">
-        <v>0.95257176450078</v>
+        <v>1.185394064502065</v>
       </c>
       <c r="F326" t="n">
         <v>0.003</v>
@@ -7954,7 +7954,7 @@
         <v>3.005395148728367</v>
       </c>
       <c r="E327" t="n">
-        <v>0.9534943591413653</v>
+        <v>1.186404140255889</v>
       </c>
       <c r="F327" t="n">
         <v>0.003</v>
@@ -7977,7 +7977,7 @@
         <v>3.005395148728367</v>
       </c>
       <c r="E328" t="n">
-        <v>0.95257176450078</v>
+        <v>1.185405064231241</v>
       </c>
       <c r="F328" t="n">
         <v>0.003</v>
@@ -8000,7 +8000,7 @@
         <v>4.004047951760818</v>
       </c>
       <c r="E329" t="n">
-        <v>0.9479619290959594</v>
+        <v>1.180387638014894</v>
       </c>
       <c r="F329" t="n">
         <v>0.004</v>
@@ -8023,7 +8023,7 @@
         <v>2.008083663595718</v>
       </c>
       <c r="E330" t="n">
-        <v>0.950727202890569</v>
+        <v>1.183406884292891</v>
       </c>
       <c r="F330" t="n">
         <v>0.002</v>
@@ -8046,7 +8046,7 @@
         <v>3.005395148728367</v>
       </c>
       <c r="E331" t="n">
-        <v>0.9498052358467118</v>
+        <v>1.182407780379059</v>
       </c>
       <c r="F331" t="n">
         <v>0.003</v>
@@ -8069,7 +8069,7 @@
         <v>3.005395148728367</v>
       </c>
       <c r="E332" t="n">
-        <v>0.9461194585471793</v>
+        <v>1.178394869548375</v>
       </c>
       <c r="F332" t="n">
         <v>0.003</v>
@@ -8115,7 +8115,7 @@
         <v>4.363714014460617</v>
       </c>
       <c r="E334" t="n">
-        <v>0.9678954363049511</v>
+        <v>1.202089294507288</v>
       </c>
       <c r="F334" t="n">
         <v>0.00436</v>
@@ -8138,7 +8138,7 @@
         <v>2.925542684699712</v>
       </c>
       <c r="E335" t="n">
-        <v>0.9516586019146699</v>
+        <v>1.184443888666523</v>
       </c>
       <c r="F335" t="n">
         <v>0.00292</v>
@@ -8161,7 +8161,7 @@
         <v>3.025359482772254</v>
       </c>
       <c r="E336" t="n">
-        <v>0.9468471345172325</v>
+        <v>1.17920528659633</v>
       </c>
       <c r="F336" t="n">
         <v>0.00302</v>
@@ -8184,7 +8184,7 @@
         <v>2.446630335788388</v>
       </c>
       <c r="E337" t="n">
-        <v>0.9515018168461145</v>
+        <v>1.184284064462546</v>
       </c>
       <c r="F337" t="n">
         <v>0.00244</v>
@@ -8207,7 +8207,7 @@
         <v>2.56632032295269</v>
       </c>
       <c r="E338" t="n">
-        <v>0.9490770297455114</v>
+        <v>1.181646995647688</v>
       </c>
       <c r="F338" t="n">
         <v>0.00256</v>
@@ -8230,7 +8230,7 @@
         <v>3.145155004129367</v>
       </c>
       <c r="E339" t="n">
-        <v>0.9510591622272271</v>
+        <v>1.183812411439786</v>
       </c>
       <c r="F339" t="n">
         <v>0.00314</v>
@@ -8253,7 +8253,7 @@
         <v>2.307032726252491</v>
       </c>
       <c r="E340" t="n">
-        <v>0.9447197399994302</v>
+        <v>1.176906022389478</v>
       </c>
       <c r="F340" t="n">
         <v>0.0023</v>
@@ -8276,7 +8276,7 @@
         <v>3.834227431960707</v>
       </c>
       <c r="E341" t="n">
-        <v>0.9461747204997389</v>
+        <v>1.178498793476506</v>
       </c>
       <c r="F341" t="n">
         <v>0.00383</v>
@@ -8299,7 +8299,7 @@
         <v>2.715971281144188</v>
       </c>
       <c r="E342" t="n">
-        <v>0.9464970968841381</v>
+        <v>1.178856065575015</v>
       </c>
       <c r="F342" t="n">
         <v>0.00271</v>
@@ -8322,7 +8322,7 @@
         <v>2.735927630621834</v>
       </c>
       <c r="E343" t="n">
-        <v>0.947602581716822</v>
+        <v>1.180067095202589</v>
       </c>
       <c r="F343" t="n">
         <v>0.00273</v>
@@ -8345,7 +8345,7 @@
         <v>3.035341825890455</v>
       </c>
       <c r="E344" t="n">
-        <v>0.9508839580881443</v>
+        <v>1.183648915657466</v>
       </c>
       <c r="F344" t="n">
         <v>0.00303</v>
@@ -8368,7 +8368,7 @@
         <v>3.065289545866752</v>
       </c>
       <c r="E345" t="n">
-        <v>0.9471972023307376</v>
+        <v>1.179635772369988</v>
       </c>
       <c r="F345" t="n">
         <v>0.00306</v>
@@ -8414,7 +8414,7 @@
         <v>2.676060537431842</v>
       </c>
       <c r="E347" t="n">
-        <v>0.9489111276227077</v>
+        <v>1.181509897514965</v>
       </c>
       <c r="F347" t="n">
         <v>0.00267</v>
@@ -8437,7 +8437,7 @@
         <v>3.005395148728367</v>
       </c>
       <c r="E348" t="n">
-        <v>0.9431640406617851</v>
+        <v>1.175246259095248</v>
       </c>
       <c r="F348" t="n">
         <v>0.003</v>
@@ -8483,7 +8483,7 @@
         <v>3.624472375394797</v>
       </c>
       <c r="E350" t="n">
-        <v>0.9449499236963195</v>
+        <v>1.177200754739034</v>
       </c>
       <c r="F350" t="n">
         <v>0.00362</v>
@@ -8552,7 +8552,7 @@
         <v>2.596247291765559</v>
       </c>
       <c r="E353" t="n">
-        <v>0.9366990992526366</v>
+        <v>1.168205089936073</v>
       </c>
       <c r="F353" t="n">
         <v>0.00259</v>
@@ -8575,7 +8575,7 @@
         <v>3.085255256862874</v>
       </c>
       <c r="E354" t="n">
-        <v>0.9514464823830062</v>
+        <v>1.184305589772814</v>
       </c>
       <c r="F354" t="n">
         <v>0.00308</v>
@@ -8644,7 +8644,7 @@
         <v>3.065289545866752</v>
       </c>
       <c r="E357" t="n">
-        <v>0.9386659979179168</v>
+        <v>1.170371357137999</v>
       </c>
       <c r="F357" t="n">
         <v>0.00306</v>
@@ -8690,7 +8690,7 @@
         <v>3.01537725666292</v>
       </c>
       <c r="E359" t="n">
-        <v>0.9421057697613661</v>
+        <v>1.174139788773147</v>
       </c>
       <c r="F359" t="n">
         <v>0.00301</v>
@@ -8713,7 +8713,7 @@
         <v>2.616199533674754</v>
       </c>
       <c r="E360" t="n">
-        <v>0.9456313439721081</v>
+        <v>1.177993263862906</v>
       </c>
       <c r="F360" t="n">
         <v>0.00261</v>
@@ -8759,7 +8759,7 @@
         <v>2.616199533674754</v>
       </c>
       <c r="E362" t="n">
-        <v>0.9414249414705006</v>
+        <v>1.173407164873664</v>
       </c>
       <c r="F362" t="n">
         <v>0.00261</v>
@@ -8805,7 +8805,7 @@
         <v>3.005395148728367</v>
       </c>
       <c r="E364" t="n">
-        <v>0.9415813378534651</v>
+        <v>1.173583396650554</v>
       </c>
       <c r="F364" t="n">
         <v>0.003</v>
@@ -8851,7 +8851,7 @@
         <v>2.646129248543994</v>
       </c>
       <c r="E366" t="n">
-        <v>0.9377927240357342</v>
+        <v>1.169449360899398</v>
       </c>
       <c r="F366" t="n">
         <v>0.00264</v>
@@ -8874,7 +8874,7 @@
         <v>2.466576574931336</v>
       </c>
       <c r="E367" t="n">
-        <v>0.9448210192173433</v>
+        <v>1.177131101751688</v>
       </c>
       <c r="F367" t="n">
         <v>0.00246</v>
@@ -8897,7 +8897,7 @@
         <v>3.664423556304593</v>
       </c>
       <c r="E368" t="n">
-        <v>0.935872184260918</v>
+        <v>1.167360692752849</v>
       </c>
       <c r="F368" t="n">
         <v>0.00366</v>
@@ -8943,7 +8943,7 @@
         <v>2.167487024182613</v>
       </c>
       <c r="E370" t="n">
-        <v>0.9407718218000085</v>
+        <v>1.172721173732192</v>
       </c>
       <c r="F370" t="n">
         <v>0.00216</v>
@@ -8966,7 +8966,7 @@
         <v>2.636152499382386</v>
       </c>
       <c r="E371" t="n">
-        <v>0.9419953574061466</v>
+        <v>1.174062729151484</v>
       </c>
       <c r="F371" t="n">
         <v>0.00263</v>
@@ -9035,7 +9035,7 @@
         <v>2.386797016924564</v>
       </c>
       <c r="E374" t="n">
-        <v>0.9444435367990087</v>
+        <v>1.176740806208471</v>
       </c>
       <c r="F374" t="n">
         <v>0.00238</v>
@@ -9058,7 +9058,7 @@
         <v>2.596247291765559</v>
       </c>
       <c r="E375" t="n">
-        <v>0.9397601540709394</v>
+        <v>1.171637510675038</v>
       </c>
       <c r="F375" t="n">
         <v>0.00259</v>
@@ -9104,7 +9104,7 @@
         <v>2.366854452643846</v>
       </c>
       <c r="E377" t="n">
-        <v>0.9462944573111804</v>
+        <v>1.178776757059871</v>
       </c>
       <c r="F377" t="n">
         <v>0.00236</v>
@@ -9127,7 +9127,7 @@
         <v>2.476550019684642</v>
       </c>
       <c r="E378" t="n">
-        <v>0.9313547009764779</v>
+        <v>1.162454960213361</v>
       </c>
       <c r="F378" t="n">
         <v>0.00247</v>
@@ -9150,7 +9150,7 @@
         <v>2.705993348107123</v>
       </c>
       <c r="E379" t="n">
-        <v>0.9315382401224647</v>
+        <v>1.162661307937529</v>
       </c>
       <c r="F379" t="n">
         <v>0.0027</v>
@@ -9196,7 +9196,7 @@
         <v>2.466576574931336</v>
       </c>
       <c r="E381" t="n">
-        <v>0.9440660894982504</v>
+        <v>1.176361606646009</v>
       </c>
       <c r="F381" t="n">
         <v>0.00246</v>
@@ -9242,7 +9242,7 @@
         <v>2.745906043549196</v>
       </c>
       <c r="E383" t="n">
-        <v>0.9380684743913706</v>
+        <v>1.169815894624075</v>
       </c>
       <c r="F383" t="n">
         <v>0.00274</v>
@@ -9265,7 +9265,7 @@
         <v>2.725949375905576</v>
       </c>
       <c r="E384" t="n">
-        <v>0.9395946324884259</v>
+        <v>1.171489265848435</v>
       </c>
       <c r="F384" t="n">
         <v>0.00272</v>
@@ -9311,7 +9311,7 @@
         <v>2.526420392571276</v>
       </c>
       <c r="E386" t="n">
-        <v>0.9325753928997967</v>
+        <v>1.16381829848461</v>
       </c>
       <c r="F386" t="n">
         <v>0.00252</v>
@@ -9334,7 +9334,7 @@
         <v>3.354832335601885</v>
       </c>
       <c r="E387" t="n">
-        <v>0.9387211583803989</v>
+        <v>1.170545775589499</v>
       </c>
       <c r="F387" t="n">
         <v>0.00335</v>
@@ -9380,7 +9380,7 @@
         <v>2.745906043549196</v>
       </c>
       <c r="E389" t="n">
-        <v>0.9322724800649581</v>
+        <v>1.163497321379804</v>
       </c>
       <c r="F389" t="n">
         <v>0.00274</v>
@@ -9426,7 +9426,7 @@
         <v>2.067849124090053</v>
       </c>
       <c r="E391" t="n">
-        <v>0.9339984690114052</v>
+        <v>1.165391751118538</v>
       </c>
       <c r="F391" t="n">
         <v>0.00206</v>
@@ -9472,7 +9472,7 @@
         <v>2.48652367774771</v>
       </c>
       <c r="E393" t="n">
-        <v>0.9308775382052039</v>
+        <v>1.161980808786116</v>
       </c>
       <c r="F393" t="n">
         <v>0.00248</v>
@@ -9495,7 +9495,7 @@
         <v>2.336942446873692</v>
       </c>
       <c r="E394" t="n">
-        <v>0.9324927780574808</v>
+        <v>1.16375467142139</v>
       </c>
       <c r="F394" t="n">
         <v>0.00233</v>
@@ -9518,7 +9518,7 @@
         <v>2.48652367774771</v>
       </c>
       <c r="E395" t="n">
-        <v>0.9291253661377883</v>
+        <v>1.160072388941223</v>
       </c>
       <c r="F395" t="n">
         <v>0.00248</v>
@@ -9587,7 +9587,7 @@
         <v>2.426684981615867</v>
       </c>
       <c r="E398" t="n">
-        <v>0.9312996408580714</v>
+        <v>1.162459200934946</v>
       </c>
       <c r="F398" t="n">
         <v>0.00242</v>
@@ -9633,7 +9633,7 @@
         <v>1.84878338374186</v>
       </c>
       <c r="E400" t="n">
-        <v>0.9330252144377854</v>
+        <v>1.164353669680067</v>
       </c>
       <c r="F400" t="n">
         <v>0.00184</v>
@@ -9656,7 +9656,7 @@
         <v>1.948332620473209</v>
       </c>
       <c r="E401" t="n">
-        <v>0.9285751024488688</v>
+        <v>1.159485636947249</v>
       </c>
       <c r="F401" t="n">
         <v>0.00194</v>
@@ -9679,7 +9679,7 @@
         <v>2.935523803344132</v>
       </c>
       <c r="E402" t="n">
-        <v>0.9322816589082951</v>
+        <v>1.163550556510426</v>
       </c>
       <c r="F402" t="n">
         <v>0.00293</v>
@@ -9702,7 +9702,7 @@
         <v>2.945505050072059</v>
       </c>
       <c r="E403" t="n">
-        <v>0.9304096063674707</v>
+        <v>1.161506078813211</v>
       </c>
       <c r="F403" t="n">
         <v>0.00294</v>
@@ -9748,7 +9748,7 @@
         <v>3.704375790872195</v>
       </c>
       <c r="E405" t="n">
-        <v>0.9291437095521167</v>
+        <v>1.160124780438368</v>
       </c>
       <c r="F405" t="n">
         <v>0.0037</v>
@@ -9771,7 +9771,7 @@
         <v>2.636152499382386</v>
       </c>
       <c r="E406" t="n">
-        <v>0.9214559571993726</v>
+        <v>1.151699466515977</v>
       </c>
       <c r="F406" t="n">
         <v>0.00263</v>
@@ -9794,7 +9794,7 @@
         <v>2.636152499382386</v>
       </c>
       <c r="E407" t="n">
-        <v>0.9298683410642911</v>
+        <v>1.160929381341113</v>
       </c>
       <c r="F407" t="n">
         <v>0.00263</v>
@@ -9863,7 +9863,7 @@
         <v>2.636152499382386</v>
       </c>
       <c r="E410" t="n">
-        <v>0.9258524011644247</v>
+        <v>1.156533481216371</v>
       </c>
       <c r="F410" t="n">
         <v>0.00263</v>
@@ -9886,7 +9886,7 @@
         <v>2.416712643240814</v>
       </c>
       <c r="E411" t="n">
-        <v>0.9364418187058192</v>
+        <v>1.168134984492253</v>
       </c>
       <c r="F411" t="n">
         <v>0.00241</v>
@@ -9909,7 +9909,7 @@
         <v>3.175106297433206</v>
       </c>
       <c r="E412" t="n">
-        <v>0.9142579883334975</v>
+        <v>1.143812519755602</v>
       </c>
       <c r="F412" t="n">
         <v>0.00317</v>
@@ -9932,7 +9932,7 @@
         <v>2.416712643240814</v>
       </c>
       <c r="E413" t="n">
-        <v>0.9302169443029801</v>
+        <v>1.161332778951133</v>
       </c>
       <c r="F413" t="n">
         <v>0.00241</v>
@@ -9978,7 +9978,7 @@
         <v>2.297063342618135</v>
       </c>
       <c r="E415" t="n">
-        <v>0.9340443830312092</v>
+        <v>1.165528510816916</v>
       </c>
       <c r="F415" t="n">
         <v>0.00229</v>
@@ -10001,7 +10001,7 @@
         <v>2.446630335788388</v>
       </c>
       <c r="E416" t="n">
-        <v>0.9319971244561482</v>
+        <v>1.163293028883454</v>
       </c>
       <c r="F416" t="n">
         <v>0.00244</v>
@@ -10024,7 +10024,7 @@
         <v>2.945505050072059</v>
       </c>
       <c r="E417" t="n">
-        <v>0.9301068558197689</v>
+        <v>1.161228357123705</v>
       </c>
       <c r="F417" t="n">
         <v>0.00294</v>
@@ -10047,7 +10047,7 @@
         <v>2.626175927084855</v>
       </c>
       <c r="E418" t="n">
-        <v>0.9277773532757608</v>
+        <v>1.158681317751118</v>
       </c>
       <c r="F418" t="n">
         <v>0.00262</v>
@@ -10070,7 +10070,7 @@
         <v>2.626175927084855</v>
       </c>
       <c r="E419" t="n">
-        <v>0.925916551443152</v>
+        <v>1.156646752302204</v>
       </c>
       <c r="F419" t="n">
         <v>0.00262</v>
@@ -10093,7 +10093,7 @@
         <v>2.606223321206377</v>
       </c>
       <c r="E420" t="n">
-        <v>0.9275023039008911</v>
+        <v>1.158390599036872</v>
       </c>
       <c r="F420" t="n">
         <v>0.0026</v>
@@ -10139,7 +10139,7 @@
         <v>1.659789143234766</v>
       </c>
       <c r="E422" t="n">
-        <v>0.9269705949146103</v>
+        <v>1.157813127803633</v>
       </c>
       <c r="F422" t="n">
         <v>0.00165</v>
@@ -10162,7 +10162,7 @@
         <v>2.686037974415105</v>
       </c>
       <c r="E423" t="n">
-        <v>0.9236352614629195</v>
+        <v>1.154160622884358</v>
       </c>
       <c r="F423" t="n">
         <v>0.00268</v>
@@ -10185,7 +10185,7 @@
         <v>3.065289545866752</v>
       </c>
       <c r="E424" t="n">
-        <v>0.9296940507256914</v>
+        <v>1.160808471739818</v>
       </c>
       <c r="F424" t="n">
         <v>0.00306</v>
@@ -10208,7 +10208,7 @@
         <v>3.01537725666292</v>
       </c>
       <c r="E425" t="n">
-        <v>0.9135087496614951</v>
+        <v>1.143046862464614</v>
       </c>
       <c r="F425" t="n">
         <v>0.00301</v>
@@ -10231,7 +10231,7 @@
         <v>2.66608326951729</v>
       </c>
       <c r="E426" t="n">
-        <v>0.9250643524078294</v>
+        <v>1.155744371082667</v>
       </c>
       <c r="F426" t="n">
         <v>0.00266</v>
@@ -10254,7 +10254,7 @@
         <v>2.66608326951729</v>
       </c>
       <c r="E427" t="n">
-        <v>0.9298591677010881</v>
+        <v>1.161005708918647</v>
       </c>
       <c r="F427" t="n">
         <v>0.00266</v>
@@ -10300,7 +10300,7 @@
         <v>2.426684981615867</v>
       </c>
       <c r="E429" t="n">
-        <v>0.9198634298550422</v>
+        <v>1.150047448724409</v>
       </c>
       <c r="F429" t="n">
         <v>0.00242</v>
@@ -10346,7 +10346,7 @@
         <v>2.267156809750927</v>
       </c>
       <c r="E431" t="n">
-        <v>0.9147971610834053</v>
+        <v>1.144485419648581</v>
       </c>
       <c r="F431" t="n">
         <v>0.00226</v>
@@ -10369,7 +10369,7 @@
         <v>2.975449545866978</v>
       </c>
       <c r="E432" t="n">
-        <v>0.9234703989403712</v>
+        <v>1.154017409307227</v>
       </c>
       <c r="F432" t="n">
         <v>0.00297</v>
@@ -10392,7 +10392,7 @@
         <v>2.995413160150032</v>
       </c>
       <c r="E433" t="n">
-        <v>0.9222616130775337</v>
+        <v>1.15269584931854</v>
       </c>
       <c r="F433" t="n">
         <v>0.00299</v>
@@ -10415,7 +10415,7 @@
         <v>3.055306858565928</v>
       </c>
       <c r="E434" t="n">
-        <v>0.9250643524078294</v>
+        <v>1.155776736691035</v>
       </c>
       <c r="F434" t="n">
         <v>0.00305</v>
@@ -10461,7 +10461,7 @@
         <v>2.646129248543994</v>
       </c>
       <c r="E436" t="n">
-        <v>0.9182898261049598</v>
+        <v>1.148345790479463</v>
       </c>
       <c r="F436" t="n">
         <v>0.00264</v>
@@ -10484,7 +10484,7 @@
         <v>2.636152499382386</v>
       </c>
       <c r="E437" t="n">
-        <v>0.917356932953998</v>
+        <v>1.147326056181215</v>
       </c>
       <c r="F437" t="n">
         <v>0.00263</v>
@@ -10507,7 +10507,7 @@
         <v>2.646129248543994</v>
       </c>
       <c r="E438" t="n">
-        <v>0.9315198858327705</v>
+        <v>1.162868179442579</v>
       </c>
       <c r="F438" t="n">
         <v>0.00264</v>
@@ -10553,7 +10553,7 @@
         <v>2.804567702873296</v>
       </c>
       <c r="E440" t="n">
-        <v>0.9280707599327939</v>
+        <v>1.15909468678074</v>
       </c>
       <c r="F440" t="n">
         <v>0.0028</v>
@@ -10576,7 +10576,7 @@
         <v>2.814551474036316</v>
       </c>
       <c r="E441" t="n">
-        <v>0.9241756914400466</v>
+        <v>1.154828530412531</v>
       </c>
       <c r="F441" t="n">
         <v>0.00281</v>
@@ -10622,7 +10622,7 @@
         <v>4.452875475465264</v>
       </c>
       <c r="E443" t="n">
-        <v>0.9188661328458655</v>
+        <v>1.149004997784165</v>
       </c>
       <c r="F443" t="n">
         <v>0.00445</v>
@@ -10645,7 +10645,7 @@
         <v>3.044207614470472</v>
       </c>
       <c r="E444" t="n">
-        <v>0.9287126613416902</v>
+        <v>1.159813926282082</v>
       </c>
       <c r="F444" t="n">
         <v>0.00304</v>
@@ -10691,7 +10691,7 @@
         <v>4.382921400162226</v>
       </c>
       <c r="E446" t="n">
-        <v>0.9268147624506331</v>
+        <v>1.157738977167178</v>
       </c>
       <c r="F446" t="n">
         <v>0.00438</v>
@@ -10714,7 +10714,7 @@
         <v>2.754650613054222</v>
       </c>
       <c r="E447" t="n">
-        <v>0.9099745928341839</v>
+        <v>1.139242388222665</v>
       </c>
       <c r="F447" t="n">
         <v>0.00275</v>
@@ -10760,7 +10760,7 @@
         <v>2.644844040770646</v>
       </c>
       <c r="E449" t="n">
-        <v>0.9213277995239002</v>
+        <v>1.151729962313207</v>
       </c>
       <c r="F449" t="n">
         <v>0.00264</v>
@@ -10783,7 +10783,7 @@
         <v>3.493665696657309</v>
       </c>
       <c r="E450" t="n">
-        <v>0.9203301398889</v>
+        <v>1.150639850927604</v>
       </c>
       <c r="F450" t="n">
         <v>0.00349</v>
@@ -10806,7 +10806,7 @@
         <v>2.205810508633958</v>
       </c>
       <c r="E451" t="n">
-        <v>0.90777530599831</v>
+        <v>1.136836173469844</v>
       </c>
       <c r="F451" t="n">
         <v>0.0022</v>
@@ -10875,7 +10875,7 @@
         <v>2.465197760829747</v>
       </c>
       <c r="E454" t="n">
-        <v>0.9234062875577276</v>
+        <v>1.154027183825306</v>
       </c>
       <c r="F454" t="n">
         <v>0.00246</v>
@@ -10898,7 +10898,7 @@
         <v>2.794584047760954</v>
       </c>
       <c r="E455" t="n">
-        <v>0.9229025907389407</v>
+        <v>1.153479777996047</v>
       </c>
       <c r="F455" t="n">
         <v>0.00279</v>
@@ -10944,7 +10944,7 @@
         <v>2.724701818548224</v>
       </c>
       <c r="E457" t="n">
-        <v>0.9164425417211464</v>
+        <v>1.146389666582425</v>
       </c>
       <c r="F457" t="n">
         <v>0.00272</v>
@@ -10967,7 +10967,7 @@
         <v>2.984292210893565</v>
       </c>
       <c r="E458" t="n">
-        <v>0.9139107628065983</v>
+        <v>1.143611058520664</v>
       </c>
       <c r="F458" t="n">
         <v>0.00298</v>
@@ -10990,7 +10990,7 @@
         <v>2.485155930721451</v>
       </c>
       <c r="E459" t="n">
-        <v>0.9200372958996209</v>
+        <v>1.150350463100592</v>
       </c>
       <c r="F459" t="n">
         <v>0.00248</v>
@@ -11013,7 +11013,7 @@
         <v>2.345463706817907</v>
       </c>
       <c r="E460" t="n">
-        <v>0.9214284944971752</v>
+        <v>1.151883839006068</v>
       </c>
       <c r="F460" t="n">
         <v>0.00234</v>
@@ -11036,7 +11036,7 @@
         <v>3.104126286090823</v>
       </c>
       <c r="E461" t="n">
-        <v>0.9141574725968361</v>
+        <v>1.143899096035312</v>
       </c>
       <c r="F461" t="n">
         <v>0.0031</v>
@@ -11059,7 +11059,7 @@
         <v>2.734684625327023</v>
       </c>
       <c r="E462" t="n">
-        <v>0.9135087496614951</v>
+        <v>1.143190819925149</v>
       </c>
       <c r="F462" t="n">
         <v>0.00273</v>
@@ -11082,7 +11082,7 @@
         <v>3.074166553718259</v>
       </c>
       <c r="E463" t="n">
-        <v>0.9189118750099009</v>
+        <v>1.149135979866623</v>
       </c>
       <c r="F463" t="n">
         <v>0.00307</v>
@@ -11105,7 +11105,7 @@
         <v>2.704736586065268</v>
       </c>
       <c r="E464" t="n">
-        <v>0.9117915099627758</v>
+        <v>1.141311921959393</v>
       </c>
       <c r="F464" t="n">
         <v>0.0027</v>
@@ -11151,7 +11151,7 @@
         <v>2.904410439314664</v>
       </c>
       <c r="E466" t="n">
-        <v>0.9154186702152899</v>
+        <v>1.145307309795001</v>
       </c>
       <c r="F466" t="n">
         <v>0.0029</v>
@@ -11197,7 +11197,7 @@
         <v>2.874456470360962</v>
       </c>
       <c r="E468" t="n">
-        <v>0.9152998448667076</v>
+        <v>1.14518196510965</v>
       </c>
       <c r="F468" t="n">
         <v>0.00287</v>
@@ -11220,7 +11220,7 @@
         <v>4.672740095490012</v>
       </c>
       <c r="E469" t="n">
-        <v>0.9162596884093841</v>
+        <v>1.146242602322948</v>
       </c>
       <c r="F469" t="n">
         <v>0.00467</v>
@@ -11266,7 +11266,7 @@
         <v>2.415305363716977</v>
       </c>
       <c r="E471" t="n">
-        <v>0.9166619766660832</v>
+        <v>1.146690153557622</v>
       </c>
       <c r="F471" t="n">
         <v>0.00241</v>
@@ -11289,7 +11289,7 @@
         <v>2.275631780407366</v>
       </c>
       <c r="E472" t="n">
-        <v>0.9153912486693963</v>
+        <v>1.145298412998866</v>
       </c>
       <c r="F472" t="n">
         <v>0.00227</v>
@@ -11335,7 +11335,7 @@
         <v>3.223972704599095</v>
       </c>
       <c r="E474" t="n">
-        <v>0.9094908288756455</v>
+        <v>1.138810881583278</v>
       </c>
       <c r="F474" t="n">
         <v>0.00322</v>
@@ -11358,7 +11358,7 @@
         <v>2.744667557282667</v>
       </c>
       <c r="E475" t="n">
-        <v>0.9138102557510883</v>
+        <v>1.143570426074773</v>
       </c>
       <c r="F475" t="n">
         <v>0.00274</v>
@@ -11381,7 +11381,7 @@
         <v>2.37539470404394</v>
       </c>
       <c r="E476" t="n">
-        <v>0.9134265246528341</v>
+        <v>1.143153590803389</v>
       </c>
       <c r="F476" t="n">
         <v>0.00237</v>
@@ -11404,7 +11404,7 @@
         <v>2.974306641891518</v>
       </c>
       <c r="E477" t="n">
-        <v>0.9153638273104667</v>
+        <v>1.145289499836079</v>
       </c>
       <c r="F477" t="n">
         <v>0.00297</v>
@@ -11427,7 +11427,7 @@
         <v>2.714719138327204</v>
       </c>
       <c r="E478" t="n">
-        <v>0.9154186702152899</v>
+        <v>1.145355105278633</v>
       </c>
       <c r="F478" t="n">
         <v>0.00271</v>
@@ -11450,7 +11450,7 @@
         <v>3.513644831225831</v>
       </c>
       <c r="E479" t="n">
-        <v>0.9074286404526959</v>
+        <v>1.136573788820807</v>
       </c>
       <c r="F479" t="n">
         <v>0.00351</v>
@@ -11496,7 +11496,7 @@
         <v>2.295582714693592</v>
       </c>
       <c r="E481" t="n">
-        <v>0.9081949938397991</v>
+        <v>1.137436317355259</v>
       </c>
       <c r="F481" t="n">
         <v>0.00229</v>
@@ -11519,7 +11519,7 @@
         <v>2.535054240050891</v>
       </c>
       <c r="E482" t="n">
-        <v>0.9115358136406398</v>
+        <v>1.141120565084683</v>
       </c>
       <c r="F482" t="n">
         <v>0.00253</v>
@@ -11542,7 +11542,7 @@
         <v>3.393773710782733</v>
       </c>
       <c r="E483" t="n">
-        <v>0.9106775235821779</v>
+        <v>1.140181013079553</v>
       </c>
       <c r="F483" t="n">
         <v>0.00339</v>
@@ -11565,7 +11565,7 @@
         <v>2.754650613054222</v>
       </c>
       <c r="E484" t="n">
-        <v>0.9131707242713692</v>
+        <v>1.142930145823856</v>
       </c>
       <c r="F484" t="n">
         <v>0.00275</v>
@@ -11588,7 +11588,7 @@
         <v>3.623534186398688</v>
       </c>
       <c r="E485" t="n">
-        <v>0.9071184914049759</v>
+        <v>1.13627129274559</v>
       </c>
       <c r="F485" t="n">
         <v>0.00362</v>
@@ -11611,7 +11611,7 @@
         <v>3.044207614470472</v>
       </c>
       <c r="E486" t="n">
-        <v>0.9080033917712333</v>
+        <v>1.137251549840165</v>
       </c>
       <c r="F486" t="n">
         <v>0.00304</v>
@@ -11634,7 +11634,7 @@
         <v>3.213985065304442</v>
       </c>
       <c r="E487" t="n">
-        <v>0.9114353659667699</v>
+        <v>1.141041488719147</v>
       </c>
       <c r="F487" t="n">
         <v>0.00321</v>
@@ -11657,7 +11657,7 @@
         <v>2.724701818548224</v>
       </c>
       <c r="E488" t="n">
-        <v>0.9095090830610814</v>
+        <v>1.138925863550574</v>
       </c>
       <c r="F488" t="n">
         <v>0.00272</v>
@@ -11680,7 +11680,7 @@
         <v>3.253936078044558</v>
       </c>
       <c r="E489" t="n">
-        <v>0.909636864683152</v>
+        <v>1.139071857557454</v>
       </c>
       <c r="F489" t="n">
         <v>0.00325</v>
@@ -11703,7 +11703,7 @@
         <v>3.33384162791216</v>
       </c>
       <c r="E490" t="n">
-        <v>0.9117093200843548</v>
+        <v>1.141358880840561</v>
       </c>
       <c r="F490" t="n">
         <v>0.00333</v>
@@ -11726,7 +11726,7 @@
         <v>2.535054240050891</v>
       </c>
       <c r="E491" t="n">
-        <v>0.9094908288756455</v>
+        <v>1.138921569430648</v>
       </c>
       <c r="F491" t="n">
         <v>0.00253</v>
@@ -11749,7 +11749,7 @@
         <v>3.014249491996308</v>
       </c>
       <c r="E492" t="n">
-        <v>0.9089158645184461</v>
+        <v>1.138293571578904</v>
       </c>
       <c r="F492" t="n">
         <v>0.00301</v>
@@ -11772,7 +11772,7 @@
         <v>3.044207614470472</v>
       </c>
       <c r="E493" t="n">
-        <v>0.9040821222710803</v>
+        <v>1.132971324080985</v>
       </c>
       <c r="F493" t="n">
         <v>0.00304</v>
@@ -11795,7 +11795,7 @@
         <v>2.525074256333861</v>
       </c>
       <c r="E494" t="n">
-        <v>0.908277111812561</v>
+        <v>1.137600468152982</v>
       </c>
       <c r="F494" t="n">
         <v>0.00252</v>
@@ -11818,7 +11818,7 @@
         <v>2.624880949681338</v>
       </c>
       <c r="E495" t="n">
-        <v>0.9060513970008159</v>
+        <v>1.135153042138041</v>
       </c>
       <c r="F495" t="n">
         <v>0.00262</v>
@@ -11841,7 +11841,7 @@
         <v>2.684771871127974</v>
       </c>
       <c r="E496" t="n">
-        <v>0.909280911708677</v>
+        <v>1.138716721426554</v>
       </c>
       <c r="F496" t="n">
         <v>0.00268</v>
@@ -11864,7 +11864,7 @@
         <v>2.564995126701024</v>
       </c>
       <c r="E497" t="n">
-        <v>0.9118554365862866</v>
+        <v>1.141556682470316</v>
       </c>
       <c r="F497" t="n">
         <v>0.00256</v>
@@ -11887,7 +11887,7 @@
         <v>2.674789711360503</v>
       </c>
       <c r="E498" t="n">
-        <v>0.9096916294804955</v>
+        <v>1.139179605740275</v>
       </c>
       <c r="F498" t="n">
         <v>0.00267</v>
@@ -11910,7 +11910,7 @@
         <v>2.624880949681338</v>
       </c>
       <c r="E499" t="n">
-        <v>0.9053948646133848</v>
+        <v>1.134450307264487</v>
       </c>
       <c r="F499" t="n">
         <v>0.00262</v>
@@ -11933,7 +11933,7 @@
         <v>2.365417510715603</v>
       </c>
       <c r="E500" t="n">
-        <v>0.9125495625482943</v>
+        <v>1.14233652672808</v>
       </c>
       <c r="F500" t="n">
         <v>0.00236</v>
@@ -11956,7 +11956,7 @@
         <v>2.60491842482639</v>
       </c>
       <c r="E501" t="n">
-        <v>0.9118554365862866</v>
+        <v>1.141577853040007</v>
       </c>
       <c r="F501" t="n">
         <v>0.0026</v>
@@ -11979,7 +11979,7 @@
         <v>3.184022612985027</v>
       </c>
       <c r="E502" t="n">
-        <v>0.9071367348028999</v>
+        <v>1.136386093415746</v>
       </c>
       <c r="F502" t="n">
         <v>0.00318</v>
@@ -12002,7 +12002,7 @@
         <v>2.185863673699712</v>
       </c>
       <c r="E503" t="n">
-        <v>0.907565478537393</v>
+        <v>1.136863827731204</v>
       </c>
       <c r="F503" t="n">
         <v>0.00218</v>
@@ -12025,7 +12025,7 @@
         <v>2.265656637710136</v>
       </c>
       <c r="E504" t="n">
-        <v>0.9137280245747393</v>
+        <v>1.143654490185253</v>
       </c>
       <c r="F504" t="n">
         <v>0.00226</v>
@@ -12071,7 +12071,7 @@
         <v>2.505114767830009</v>
       </c>
       <c r="E506" t="n">
-        <v>0.9084231034687238</v>
+        <v>1.137819309587977</v>
       </c>
       <c r="F506" t="n">
         <v>0.0025</v>
@@ -12094,7 +12094,7 @@
         <v>2.445240274492468</v>
       </c>
       <c r="E507" t="n">
-        <v>0.9063158640240818</v>
+        <v>1.135502456680003</v>
       </c>
       <c r="F507" t="n">
         <v>0.00244</v>
@@ -12117,7 +12117,7 @@
         <v>2.215784285529618</v>
       </c>
       <c r="E508" t="n">
-        <v>0.9052216309357585</v>
+        <v>1.134301417101528</v>
       </c>
       <c r="F508" t="n">
         <v>0.00221</v>
@@ -12163,7 +12163,7 @@
         <v>2.385372088375313</v>
       </c>
       <c r="E510" t="n">
-        <v>0.9051395754902748</v>
+        <v>1.134216206383758</v>
       </c>
       <c r="F510" t="n">
         <v>0.00238</v>
@@ -12186,7 +12186,7 @@
         <v>2.365417510715603</v>
       </c>
       <c r="E511" t="n">
-        <v>0.9041094666854979</v>
+        <v>1.133085518260362</v>
       </c>
       <c r="F511" t="n">
         <v>0.00236</v>
@@ -12209,7 +12209,7 @@
         <v>2.924380276229478</v>
       </c>
       <c r="E512" t="n">
-        <v>0.9001009448613514</v>
+        <v>1.128667584704442</v>
       </c>
       <c r="F512" t="n">
         <v>0.00292</v>
@@ -12232,7 +12232,7 @@
         <v>2.505114767830009</v>
       </c>
       <c r="E513" t="n">
-        <v>0.9033256674473877</v>
+        <v>1.132231495856973</v>
       </c>
       <c r="F513" t="n">
         <v>0.0025</v>
@@ -12278,7 +12278,7 @@
         <v>2.854487694841231</v>
       </c>
       <c r="E515" t="n">
-        <v>0.9093082915862332</v>
+        <v>1.138831385489395</v>
       </c>
       <c r="F515" t="n">
         <v>0.00285</v>
@@ -12301,7 +12301,7 @@
         <v>4.123105625617661</v>
       </c>
       <c r="E516" t="n">
-        <v>0.9067262784154501</v>
+        <v>1.135991713861719</v>
       </c>
       <c r="F516" t="n">
         <v>0.00412</v>
@@ -12347,7 +12347,7 @@
         <v>2.564995126701024</v>
       </c>
       <c r="E518" t="n">
-        <v>0.9089432419061898</v>
+        <v>1.138439837436215</v>
       </c>
       <c r="F518" t="n">
         <v>0.00256</v>
@@ -12370,7 +12370,7 @@
         <v>2.974306641891518</v>
       </c>
       <c r="E519" t="n">
-        <v>0.9028335927796735</v>
+        <v>1.131709650054612</v>
       </c>
       <c r="F519" t="n">
         <v>0.00297</v>
@@ -12393,7 +12393,7 @@
         <v>2.405327420539665</v>
       </c>
       <c r="E520" t="n">
-        <v>0.9049481193148058</v>
+        <v>1.134047193583685</v>
       </c>
       <c r="F520" t="n">
         <v>0.0024</v>
@@ -12439,7 +12439,7 @@
         <v>2.944350522611056</v>
       </c>
       <c r="E522" t="n">
-        <v>0.9044831923798266</v>
+        <v>1.133539750536721</v>
       </c>
       <c r="F522" t="n">
         <v>0.00294</v>
@@ -12462,7 +12462,7 @@
         <v>2.644844040770646</v>
       </c>
       <c r="E523" t="n">
-        <v>0.9042826523090505</v>
+        <v>1.13332384205636</v>
       </c>
       <c r="F523" t="n">
         <v>0.00264</v>
@@ -12485,7 +12485,7 @@
         <v>2.485155930721451</v>
       </c>
       <c r="E524" t="n">
-        <v>0.9043282287168695</v>
+        <v>1.133379365948628</v>
       </c>
       <c r="F524" t="n">
         <v>0.00248</v>
@@ -12508,7 +12508,7 @@
         <v>2.654825794661488</v>
       </c>
       <c r="E525" t="n">
-        <v>0.8993907617797346</v>
+        <v>1.127935804925749</v>
       </c>
       <c r="F525" t="n">
         <v>0.00265</v>
@@ -12531,7 +12531,7 @@
         <v>3.84333188782858</v>
       </c>
       <c r="E526" t="n">
-        <v>0.9063341037719762</v>
+        <v>1.135601591244408</v>
       </c>
       <c r="F526" t="n">
         <v>0.00384</v>
@@ -12554,7 +12554,7 @@
         <v>2.904410439314664</v>
       </c>
       <c r="E527" t="n">
-        <v>0.8965058012632641</v>
+        <v>1.124759386194893</v>
       </c>
       <c r="F527" t="n">
         <v>0.0029</v>
@@ -12577,7 +12577,7 @@
         <v>2.495135266874323</v>
       </c>
       <c r="E528" t="n">
-        <v>0.896787834968613</v>
+        <v>1.125076257409196</v>
       </c>
       <c r="F528" t="n">
         <v>0.00249</v>
@@ -12600,7 +12600,7 @@
         <v>2.684771871127974</v>
       </c>
       <c r="E529" t="n">
-        <v>0.9015399070209057</v>
+        <v>1.130329330889188</v>
       </c>
       <c r="F529" t="n">
         <v>0.00268</v>
@@ -12623,7 +12623,7 @@
         <v>2.33</v>
       </c>
       <c r="E530" t="n">
-        <v>0.9029702741256218</v>
+        <v>1.131912959970071</v>
       </c>
       <c r="F530" t="n">
         <v>0.00233</v>
@@ -12646,7 +12646,7 @@
         <v>2.68</v>
       </c>
       <c r="E531" t="n">
-        <v>0.8980981878398632</v>
+        <v>1.126539614624197</v>
       </c>
       <c r="F531" t="n">
         <v>0.00268</v>
@@ -12669,7 +12669,7 @@
         <v>2.24</v>
       </c>
       <c r="E532" t="n">
-        <v>0.8967150501726771</v>
+        <v>1.125016709547205</v>
       </c>
       <c r="F532" t="n">
         <v>0.00224</v>
@@ -12692,7 +12692,7 @@
         <v>2.68</v>
       </c>
       <c r="E533" t="n">
-        <v>0.8994818038512747</v>
+        <v>1.128078207173131</v>
       </c>
       <c r="F533" t="n">
         <v>0.00268</v>
@@ -12715,7 +12715,7 @@
         <v>2.7</v>
       </c>
       <c r="E534" t="n">
-        <v>0.9005289365331069</v>
+        <v>1.129244843535206</v>
       </c>
       <c r="F534" t="n">
         <v>0.0027</v>
@@ -12738,7 +12738,7 @@
         <v>2.68</v>
       </c>
       <c r="E535" t="n">
-        <v>0.9078117988507551</v>
+        <v>1.137282977730266</v>
       </c>
       <c r="F535" t="n">
         <v>0.00268</v>
@@ -12761,7 +12761,7 @@
         <v>3.01</v>
       </c>
       <c r="E536" t="n">
-        <v>0.9024600208904852</v>
+        <v>1.131386713487031</v>
       </c>
       <c r="F536" t="n">
         <v>0.00301</v>
@@ -12784,7 +12784,7 @@
         <v>3.45</v>
       </c>
       <c r="E537" t="n">
-        <v>0.9013668399124728</v>
+        <v>1.130185509285349</v>
       </c>
       <c r="F537" t="n">
         <v>0.00345</v>
@@ -12807,7 +12807,7 @@
         <v>3.02</v>
       </c>
       <c r="E538" t="n">
-        <v>0.8993179296135654</v>
+        <v>1.127928642223044</v>
       </c>
       <c r="F538" t="n">
         <v>0.00302</v>
@@ -12830,7 +12830,7 @@
         <v>2.74</v>
       </c>
       <c r="E539" t="n">
-        <v>0.9002284269576439</v>
+        <v>1.128939262679997</v>
       </c>
       <c r="F539" t="n">
         <v>0.00274</v>
@@ -12853,7 +12853,7 @@
         <v>2.72</v>
       </c>
       <c r="E540" t="n">
-        <v>0.8999370452740311</v>
+        <v>1.12862277519433</v>
       </c>
       <c r="F540" t="n">
         <v>0.00272</v>
@@ -12876,7 +12876,7 @@
         <v>2.71</v>
       </c>
       <c r="E541" t="n">
-        <v>0.8977523585833398</v>
+        <v>1.126215059911492</v>
       </c>
       <c r="F541" t="n">
         <v>0.00271</v>
@@ -12899,7 +12899,7 @@
         <v>2.64</v>
       </c>
       <c r="E542" t="n">
-        <v>0.8967332462474702</v>
+        <v>1.125094235824559</v>
       </c>
       <c r="F542" t="n">
         <v>0.00264</v>
@@ -12922,7 +12922,7 @@
         <v>2.51</v>
       </c>
       <c r="E543" t="n">
-        <v>0.898152795192185</v>
+        <v>1.126667889085354</v>
       </c>
       <c r="F543" t="n">
         <v>0.00251</v>
@@ -12945,7 +12945,7 @@
         <v>2.27</v>
       </c>
       <c r="E544" t="n">
-        <v>0.8996912084751504</v>
+        <v>1.128372260295935</v>
       </c>
       <c r="F544" t="n">
         <v>0.00227</v>
@@ -12968,7 +12968,7 @@
         <v>2.72</v>
       </c>
       <c r="E545" t="n">
-        <v>0.8972336707501046</v>
+        <v>1.125662874504715</v>
       </c>
       <c r="F545" t="n">
         <v>0.00272</v>
@@ -12991,7 +12991,7 @@
         <v>2.41</v>
       </c>
       <c r="E546" t="n">
-        <v>0.8928320835220462</v>
+        <v>1.120801865005439</v>
       </c>
       <c r="F546" t="n">
         <v>0.00241</v>
@@ -13014,7 +13014,7 @@
         <v>2.65</v>
       </c>
       <c r="E547" t="n">
-        <v>0.9012575382237127</v>
+        <v>1.130117296451583</v>
       </c>
       <c r="F547" t="n">
         <v>0.00265</v>
@@ -13037,7 +13037,7 @@
         <v>2.62</v>
       </c>
       <c r="E548" t="n">
-        <v>0.8958144479459719</v>
+        <v>1.124110073165161</v>
       </c>
       <c r="F548" t="n">
         <v>0.00262</v>
@@ -13060,7 +13060,7 @@
         <v>2.23</v>
       </c>
       <c r="E549" t="n">
-        <v>0.8999643614059059</v>
+        <v>1.128700067144964</v>
       </c>
       <c r="F549" t="n">
         <v>0.00223</v>
@@ -13083,7 +13083,7 @@
         <v>1.95</v>
       </c>
       <c r="E550" t="n">
-        <v>0.8966604624450577</v>
+        <v>1.125055562057852</v>
       </c>
       <c r="F550" t="n">
         <v>0.00195</v>
@@ -13106,7 +13106,7 @@
         <v>3.04</v>
       </c>
       <c r="E551" t="n">
-        <v>0.8968515227517362</v>
+        <v>1.125277145935242</v>
       </c>
       <c r="F551" t="n">
         <v>0.00304</v>
@@ -13129,7 +13129,7 @@
         <v>3.02</v>
       </c>
       <c r="E552" t="n">
-        <v>0.8994089700283682</v>
+        <v>1.12811030551145</v>
       </c>
       <c r="F552" t="n">
         <v>0.00302</v>
@@ -13152,7 +13152,7 @@
         <v>2.28</v>
       </c>
       <c r="E553" t="n">
-        <v>0.9001009448613514</v>
+        <v>1.128882307647171</v>
       </c>
       <c r="F553" t="n">
         <v>0.00228</v>
@@ -13175,7 +13175,7 @@
         <v>2.62</v>
       </c>
       <c r="E554" t="n">
-        <v>0.8994909081723306</v>
+        <v>1.128213882728053</v>
       </c>
       <c r="F554" t="n">
         <v>0.00262</v>
@@ -13198,7 +13198,7 @@
         <v>2.31</v>
       </c>
       <c r="E555" t="n">
-        <v>0.8977978607248778</v>
+        <v>1.126348940861301</v>
       </c>
       <c r="F555" t="n">
         <v>0.00231</v>
@@ -13221,7 +13221,7 @@
         <v>2.68</v>
       </c>
       <c r="E556" t="n">
-        <v>0.8962601752099653</v>
+        <v>1.124654912560817</v>
       </c>
       <c r="F556" t="n">
         <v>0.00268</v>
@@ -13244,7 +13244,7 @@
         <v>2.31</v>
       </c>
       <c r="E557" t="n">
-        <v>0.8961874000176457</v>
+        <v>1.124579692160353</v>
       </c>
       <c r="F557" t="n">
         <v>0.00231</v>
@@ -13267,7 +13267,7 @@
         <v>2.41</v>
       </c>
       <c r="E558" t="n">
-        <v>0.8941593245265054</v>
+        <v>1.122342677880917</v>
       </c>
       <c r="F558" t="n">
         <v>0.00241</v>
@@ -13290,7 +13290,7 @@
         <v>2.1</v>
       </c>
       <c r="E559" t="n">
-        <v>0.8949231424777959</v>
+        <v>1.123192496671978</v>
       </c>
       <c r="F559" t="n">
         <v>0.0021</v>
@@ -13313,7 +13313,7 @@
         <v>2.92</v>
       </c>
       <c r="E560" t="n">
-        <v>0.8969789013607362</v>
+        <v>1.125470125542317</v>
       </c>
       <c r="F560" t="n">
         <v>0.00292</v>
@@ -13336,7 +13336,7 @@
         <v>1.89</v>
       </c>
       <c r="E561" t="n">
-        <v>0.9006928603545351</v>
+        <v>1.129577784039494</v>
       </c>
       <c r="F561" t="n">
         <v>0.00189</v>
@@ -13359,7 +13359,7 @@
         <v>2.81</v>
       </c>
       <c r="E562" t="n">
-        <v>0.8932320275445993</v>
+        <v>1.121337893352746</v>
       </c>
       <c r="F562" t="n">
         <v>0.00281</v>
@@ -13382,7 +13382,7 @@
         <v>1.89</v>
       </c>
       <c r="E563" t="n">
-        <v>0.898635192509575</v>
+        <v>1.1273158165838</v>
       </c>
       <c r="F563" t="n">
         <v>0.00189</v>
@@ -13405,7 +13405,7 @@
         <v>3.43</v>
       </c>
       <c r="E564" t="n">
-        <v>0.8910873417874691</v>
+        <v>1.118975287574452</v>
       </c>
       <c r="F564" t="n">
         <v>0.00343</v>
@@ -13428,7 +13428,7 @@
         <v>2.74</v>
       </c>
       <c r="E565" t="n">
-        <v>0.8918505724963898</v>
+        <v>1.119825114254539</v>
       </c>
       <c r="F565" t="n">
         <v>0.00274</v>
@@ -13451,7 +13451,7 @@
         <v>2.68</v>
       </c>
       <c r="E566" t="n">
-        <v>0.8939593010909749</v>
+        <v>1.122163122112452</v>
       </c>
       <c r="F566" t="n">
         <v>0.00268</v>
@@ -13474,7 +13474,7 @@
         <v>2.74</v>
       </c>
       <c r="E567" t="n">
-        <v>0.89185965945506</v>
+        <v>1.119845560815873</v>
       </c>
       <c r="F567" t="n">
         <v>0.00274</v>
@@ -13497,7 +13497,7 @@
         <v>2.68</v>
       </c>
       <c r="E568" t="n">
-        <v>0.8903696745982864</v>
+        <v>1.118201684323436</v>
       </c>
       <c r="F568" t="n">
         <v>0.00268</v>
@@ -13520,7 +13520,7 @@
         <v>2.52</v>
       </c>
       <c r="E569" t="n">
-        <v>0.8936956491331928</v>
+        <v>1.12188713603898</v>
       </c>
       <c r="F569" t="n">
         <v>0.00252</v>
@@ -13543,7 +13543,7 @@
         <v>3.99</v>
       </c>
       <c r="E570" t="n">
-        <v>0.8889165666738209</v>
+        <v>1.11660319467305</v>
       </c>
       <c r="F570" t="n">
         <v>0.00399</v>
@@ -13566,7 +13566,7 @@
         <v>3.77</v>
       </c>
       <c r="E571" t="n">
-        <v>0.8954051503505362</v>
+        <v>1.123787972637527</v>
       </c>
       <c r="F571" t="n">
         <v>0.00377</v>
@@ -13589,7 +13589,7 @@
         <v>3.06</v>
       </c>
       <c r="E572" t="n">
-        <v>0.8924412678233382</v>
+        <v>1.120515277689086</v>
       </c>
       <c r="F572" t="n">
         <v>0.00306</v>
@@ -13612,7 +13612,7 @@
         <v>2.44</v>
       </c>
       <c r="E573" t="n">
-        <v>0.8920504903639777</v>
+        <v>1.120087902128438</v>
       </c>
       <c r="F573" t="n">
         <v>0.00244</v>
@@ -13635,7 +13635,7 @@
         <v>2.73</v>
       </c>
       <c r="E574" t="n">
-        <v>0.8885352135185433</v>
+        <v>1.116201582423233</v>
       </c>
       <c r="F574" t="n">
         <v>0.00273</v>
@@ -13658,7 +13658,7 @@
         <v>4.52</v>
       </c>
       <c r="E575" t="n">
-        <v>0.8924776211588848</v>
+        <v>1.120570911171228</v>
       </c>
       <c r="F575" t="n">
         <v>0.00452</v>
@@ -13681,7 +13681,7 @@
         <v>2.99</v>
       </c>
       <c r="E576" t="n">
-        <v>0.8931138580974644</v>
+        <v>1.121280008679636</v>
       </c>
       <c r="F576" t="n">
         <v>0.00299</v>
@@ -13704,7 +13704,7 @@
         <v>3.92</v>
       </c>
       <c r="E577" t="n">
-        <v>0.8960145642444374</v>
+        <v>1.124492991581589</v>
       </c>
       <c r="F577" t="n">
         <v>0.00392</v>
@@ -13727,7 +13727,7 @@
         <v>2.75</v>
       </c>
       <c r="E578" t="n">
-        <v>0.8985077611505463</v>
+        <v>1.12725349395067</v>
       </c>
       <c r="F578" t="n">
         <v>0.00275</v>
@@ -13750,7 +13750,7 @@
         <v>2.96</v>
       </c>
       <c r="E579" t="n">
-        <v>0.893513830333067</v>
+        <v>1.121738062250316</v>
       </c>
       <c r="F579" t="n">
         <v>0.00296</v>
@@ -13773,7 +13773,7 @@
         <v>2.46</v>
       </c>
       <c r="E580" t="n">
-        <v>0.8968697194474896</v>
+        <v>1.125453871539575</v>
       </c>
       <c r="F580" t="n">
         <v>0.00246</v>
@@ -13796,7 +13796,7 @@
         <v>3.63</v>
       </c>
       <c r="E581" t="n">
-        <v>0.8960327571318938</v>
+        <v>1.124533933959466</v>
       </c>
       <c r="F581" t="n">
         <v>0.00363</v>
@@ -13819,7 +13819,7 @@
         <v>2.11</v>
       </c>
       <c r="E582" t="n">
-        <v>0.8937774702927764</v>
+        <v>1.122045256349135</v>
       </c>
       <c r="F582" t="n">
         <v>0.00211</v>
@@ -13842,7 +13842,7 @@
         <v>2.44</v>
       </c>
       <c r="E583" t="n">
-        <v>0.8918869204551426</v>
+        <v>1.119958796390004</v>
       </c>
       <c r="F583" t="n">
         <v>0.00244</v>
@@ -13865,7 +13865,7 @@
         <v>2.12</v>
       </c>
       <c r="E584" t="n">
-        <v>0.8911055122517177</v>
+        <v>1.119099156927143</v>
       </c>
       <c r="F584" t="n">
         <v>0.00212</v>
@@ -13888,7 +13888,7 @@
         <v>2.2</v>
       </c>
       <c r="E585" t="n">
-        <v>0.8950413654440363</v>
+        <v>1.123458630936835</v>
       </c>
       <c r="F585" t="n">
         <v>0.0022</v>
@@ -13911,7 +13911,7 @@
         <v>2.42</v>
       </c>
       <c r="E586" t="n">
-        <v>0.8917142705977635</v>
+        <v>1.119783090597261</v>
       </c>
       <c r="F586" t="n">
         <v>0.00242</v>
@@ -13934,7 +13934,7 @@
         <v>5.03</v>
       </c>
       <c r="E587" t="n">
-        <v>0.8884081039010515</v>
+        <v>1.11612873647732</v>
       </c>
       <c r="F587" t="n">
         <v>0.005030000000000001</v>
@@ -13957,7 +13957,7 @@
         <v>3.6</v>
       </c>
       <c r="E588" t="n">
-        <v>0.8927411927377192</v>
+        <v>1.120930735368503</v>
       </c>
       <c r="F588" t="n">
         <v>0.0036</v>
@@ -13980,7 +13980,7 @@
         <v>2.76</v>
       </c>
       <c r="E589" t="n">
-        <v>0.8905786023646438</v>
+        <v>1.118541782341228</v>
       </c>
       <c r="F589" t="n">
         <v>0.00276</v>
@@ -14003,7 +14003,7 @@
         <v>3.35</v>
       </c>
       <c r="E590" t="n">
-        <v>0.8888166849428992</v>
+        <v>1.116597134335108</v>
       </c>
       <c r="F590" t="n">
         <v>0.00335</v>
@@ -14026,7 +14026,7 @@
         <v>3.14</v>
       </c>
       <c r="E591" t="n">
-        <v>0.8901062595235348</v>
+        <v>1.118029385843644</v>
       </c>
       <c r="F591" t="n">
         <v>0.00314</v>
@@ -14049,7 +14049,7 @@
         <v>2.09</v>
       </c>
       <c r="E592" t="n">
-        <v>0.8899336866595117</v>
+        <v>1.11784330192502</v>
       </c>
       <c r="F592" t="n">
         <v>0.00209</v>
@@ -14072,7 +14072,7 @@
         <v>3.6</v>
       </c>
       <c r="E593" t="n">
-        <v>0.8871190780752404</v>
+        <v>1.114730964480661</v>
       </c>
       <c r="F593" t="n">
         <v>0.0036</v>
@@ -14095,7 +14095,7 @@
         <v>3.84</v>
       </c>
       <c r="E594" t="n">
-        <v>0.8897338747711243</v>
+        <v>1.117632402834827</v>
       </c>
       <c r="F594" t="n">
         <v>0.00384</v>
@@ -14118,7 +14118,7 @@
         <v>3.6</v>
       </c>
       <c r="E595" t="n">
-        <v>0.8906149387447182</v>
+        <v>1.118613061998441</v>
       </c>
       <c r="F595" t="n">
         <v>0.0036</v>
@@ -14141,7 +14141,7 @@
         <v>2.85</v>
       </c>
       <c r="E596" t="n">
-        <v>0.8859847170028731</v>
+        <v>1.113489360334337</v>
       </c>
       <c r="F596" t="n">
         <v>0.00285</v>
@@ -14164,7 +14164,7 @@
         <v>3</v>
       </c>
       <c r="E597" t="n">
-        <v>0.8830640891849477</v>
+        <v>1.110256265016121</v>
       </c>
       <c r="F597" t="n">
         <v>0.003</v>
@@ -14187,7 +14187,7 @@
         <v>3.59</v>
       </c>
       <c r="E598" t="n">
-        <v>0.8889528879232498</v>
+        <v>1.11678821060202</v>
       </c>
       <c r="F598" t="n">
         <v>0.00359</v>
@@ -14210,7 +14210,7 @@
         <v>3.57</v>
       </c>
       <c r="E599" t="n">
-        <v>0.8884534997280498</v>
+        <v>1.116240256069977</v>
       </c>
       <c r="F599" t="n">
         <v>0.00357</v>
@@ -14233,7 +14233,7 @@
         <v>4.28</v>
       </c>
       <c r="E600" t="n">
-        <v>0.8920777526668492</v>
+        <v>1.120258087576981</v>
       </c>
       <c r="F600" t="n">
         <v>0.00428</v>
@@ -14256,7 +14256,7 @@
         <v>4</v>
       </c>
       <c r="E601" t="n">
-        <v>0.8876001446170083</v>
+        <v>1.115305241404956</v>
       </c>
       <c r="F601" t="n">
         <v>0.004</v>
@@ -14279,7 +14279,7 @@
         <v>3.53</v>
       </c>
       <c r="E602" t="n">
-        <v>0.8840525092145982</v>
+        <v>1.11137815335178</v>
       </c>
       <c r="F602" t="n">
         <v>0.00353</v>
@@ -14302,7 +14302,7 @@
         <v>3.85</v>
       </c>
       <c r="E603" t="n">
-        <v>0.8815955143752102</v>
+        <v>1.108657862725088</v>
       </c>
       <c r="F603" t="n">
         <v>0.00385</v>
@@ -14325,7 +14325,7 @@
         <v>5.9</v>
       </c>
       <c r="E604" t="n">
-        <v>0.8867378967488379</v>
+        <v>1.114365308541341</v>
       </c>
       <c r="F604" t="n">
         <v>0.005900000000000001</v>
@@ -14348,7 +14348,7 @@
         <v>3.38</v>
       </c>
       <c r="E605" t="n">
-        <v>0.8770662908532949</v>
+        <v>1.103639609693116</v>
       </c>
       <c r="F605" t="n">
         <v>0.00338</v>
@@ -14371,7 +14371,7 @@
         <v>2.73</v>
       </c>
       <c r="E606" t="n">
-        <v>0.8803721157654527</v>
+        <v>1.107315567374486</v>
       </c>
       <c r="F606" t="n">
         <v>0.00273</v>
@@ -14394,7 +14394,7 @@
         <v>2.38</v>
       </c>
       <c r="E607" t="n">
-        <v>0.8855764260259114</v>
+        <v>1.113098664701003</v>
       </c>
       <c r="F607" t="n">
         <v>0.00238</v>
@@ -14417,7 +14417,7 @@
         <v>3.49</v>
       </c>
       <c r="E608" t="n">
-        <v>0.8851228184363844</v>
+        <v>1.112600967722541</v>
       </c>
       <c r="F608" t="n">
         <v>0.00349</v>
@@ -14440,7 +14440,7 @@
         <v>3.22</v>
       </c>
       <c r="E609" t="n">
-        <v>0.886501945618182</v>
+        <v>1.114134835594129</v>
       </c>
       <c r="F609" t="n">
         <v>0.00322</v>
@@ -14463,7 +14463,7 @@
         <v>3.49</v>
       </c>
       <c r="E610" t="n">
-        <v>0.8886714068891337</v>
+        <v>1.116548885042922</v>
       </c>
       <c r="F610" t="n">
         <v>0.00349</v>
@@ -14486,7 +14486,7 @@
         <v>2.96</v>
       </c>
       <c r="E611" t="n">
-        <v>0.8884444205213204</v>
+        <v>1.116307809396949</v>
       </c>
       <c r="F611" t="n">
         <v>0.00296</v>
@@ -14509,7 +14509,7 @@
         <v>1.68</v>
       </c>
       <c r="E612" t="n">
-        <v>0.8866562197771497</v>
+        <v>1.114331659628707</v>
       </c>
       <c r="F612" t="n">
         <v>0.00168</v>
@@ -14532,7 +14532,7 @@
         <v>2.68</v>
       </c>
       <c r="E613" t="n">
-        <v>0.8839346113740248</v>
+        <v>1.111319563365635</v>
       </c>
       <c r="F613" t="n">
         <v>0.00268</v>
@@ -14555,7 +14555,7 @@
         <v>2.73</v>
       </c>
       <c r="E614" t="n">
-        <v>0.8894705016583095</v>
+        <v>1.117465226188556</v>
       </c>
       <c r="F614" t="n">
         <v>0.00273</v>
@@ -14578,7 +14578,7 @@
         <v>1.69</v>
       </c>
       <c r="E615" t="n">
-        <v>0.8782705609064959</v>
+        <v>1.105054099844264</v>
       </c>
       <c r="F615" t="n">
         <v>0.00169</v>
@@ -14601,7 +14601,7 @@
         <v>2.22</v>
       </c>
       <c r="E616" t="n">
-        <v>0.8875638356834346</v>
+        <v>1.115373634614346</v>
       </c>
       <c r="F616" t="n">
         <v>0.00222</v>
@@ -14624,7 +14624,7 @@
         <v>2.3</v>
       </c>
       <c r="E617" t="n">
-        <v>0.8800459396460993</v>
+        <v>1.107045962276631</v>
       </c>
       <c r="F617" t="n">
         <v>0.0023</v>
@@ -14647,7 +14647,7 @@
         <v>2.32</v>
       </c>
       <c r="E618" t="n">
-        <v>0.8833270393732301</v>
+        <v>1.110697238709104</v>
       </c>
       <c r="F618" t="n">
         <v>0.00232</v>
@@ -14670,7 +14670,7 @@
         <v>2.32</v>
       </c>
       <c r="E619" t="n">
-        <v>0.8852226076761718</v>
+        <v>1.11280969126439</v>
       </c>
       <c r="F619" t="n">
         <v>0.00232</v>
@@ -14693,7 +14693,7 @@
         <v>2.2</v>
       </c>
       <c r="E620" t="n">
-        <v>0.8869829377038156</v>
+        <v>1.11477149452893</v>
       </c>
       <c r="F620" t="n">
         <v>0.0022</v>
@@ -14716,7 +14716,7 @@
         <v>1.71</v>
       </c>
       <c r="E621" t="n">
-        <v>0.8829915542572018</v>
+        <v>1.110356001611886</v>
       </c>
       <c r="F621" t="n">
         <v>0.00171</v>
@@ -14739,7 +14739,7 @@
         <v>2.31</v>
       </c>
       <c r="E622" t="n">
-        <v>0.8817405346940257</v>
+        <v>1.108978246568668</v>
       </c>
       <c r="F622" t="n">
         <v>0.00231</v>
@@ -14762,7 +14762,7 @@
         <v>2.58</v>
       </c>
       <c r="E623" t="n">
-        <v>0.8819036888678756</v>
+        <v>1.109169589990172</v>
       </c>
       <c r="F623" t="n">
         <v>0.00258</v>
@@ -14785,7 +14785,7 @@
         <v>2.42</v>
       </c>
       <c r="E624" t="n">
-        <v>0.8833814450280769</v>
+        <v>1.11081943116274</v>
       </c>
       <c r="F624" t="n">
         <v>0.00242</v>
@@ -14808,7 +14808,7 @@
         <v>2.28</v>
       </c>
       <c r="E625" t="n">
-        <v>0.8777272360223137</v>
+        <v>1.104553125881395</v>
       </c>
       <c r="F625" t="n">
         <v>0.00228</v>
@@ -14831,7 +14831,7 @@
         <v>2.56</v>
       </c>
       <c r="E626" t="n">
-        <v>0.8811876730526677</v>
+        <v>1.108405824841365</v>
       </c>
       <c r="F626" t="n">
         <v>0.00256</v>
@@ -14854,7 +14854,7 @@
         <v>2.37</v>
       </c>
       <c r="E627" t="n">
-        <v>0.876088655689982</v>
+        <v>1.102752971219605</v>
       </c>
       <c r="F627" t="n">
         <v>0.00237</v>
@@ -14877,7 +14877,7 @@
         <v>2.76</v>
       </c>
       <c r="E628" t="n">
-        <v>0.8876999958889192</v>
+        <v>1.115648725064717</v>
       </c>
       <c r="F628" t="n">
         <v>0.00276</v>
@@ -14900,7 +14900,7 @@
         <v>2.39</v>
       </c>
       <c r="E629" t="n">
-        <v>0.8779807783959783</v>
+        <v>1.104875961177626</v>
       </c>
       <c r="F629" t="n">
         <v>0.00239</v>
@@ -14923,7 +14923,7 @@
         <v>2.46</v>
       </c>
       <c r="E630" t="n">
-        <v>0.881097047322563</v>
+        <v>1.10834637530247</v>
       </c>
       <c r="F630" t="n">
         <v>0.00246</v>
@@ -14946,7 +14946,7 @@
         <v>3.64</v>
       </c>
       <c r="E631" t="n">
-        <v>0.8863023055684395</v>
+        <v>1.114125491622183</v>
       </c>
       <c r="F631" t="n">
         <v>0.00364</v>
@@ -14969,7 +14969,7 @@
         <v>1.62</v>
       </c>
       <c r="E632" t="n">
-        <v>0.8759890952314288</v>
+        <v>1.102683434407035</v>
       </c>
       <c r="F632" t="n">
         <v>0.00162</v>
@@ -14992,7 +14992,7 @@
         <v>1.69</v>
       </c>
       <c r="E633" t="n">
-        <v>0.8771749318273265</v>
+        <v>1.104011255890619</v>
       </c>
       <c r="F633" t="n">
         <v>0.00169</v>
@@ -15015,7 +15015,7 @@
         <v>1.76</v>
       </c>
       <c r="E634" t="n">
-        <v>0.8771115575649734</v>
+        <v>1.103951084487381</v>
       </c>
       <c r="F634" t="n">
         <v>0.00176</v>
@@ -15038,7 +15038,7 @@
         <v>1.5</v>
       </c>
       <c r="E635" t="n">
-        <v>0.8738446256366272</v>
+        <v>1.100329843646787</v>
       </c>
       <c r="F635" t="n">
         <v>0.0015</v>
@@ -15061,7 +15061,7 @@
         <v>1.91</v>
       </c>
       <c r="E636" t="n">
-        <v>0.878333953645777</v>
+        <v>1.105329619653616</v>
       </c>
       <c r="F636" t="n">
         <v>0.00191</v>
@@ -15084,7 +15084,7 @@
         <v>1.91</v>
       </c>
       <c r="E637" t="n">
-        <v>0.8760796046361303</v>
+        <v>1.10283501077169</v>
       </c>
       <c r="F637" t="n">
         <v>0.00191</v>
@@ -15107,7 +15107,7 @@
         <v>2.25</v>
       </c>
       <c r="E638" t="n">
-        <v>0.8769304938110779</v>
+        <v>1.103790865114968</v>
       </c>
       <c r="F638" t="n">
         <v>0.00225</v>
@@ -15130,7 +15130,7 @@
         <v>2.21</v>
       </c>
       <c r="E639" t="n">
-        <v>0.8775733074689694</v>
+        <v>1.104515359675289</v>
       </c>
       <c r="F639" t="n">
         <v>0.00221</v>
@@ -15153,7 +15153,7 @@
         <v>2.1</v>
       </c>
       <c r="E640" t="n">
-        <v>0.8725964803467116</v>
+        <v>1.098992619074294</v>
       </c>
       <c r="F640" t="n">
         <v>0.0021</v>
@@ -15176,7 +15176,7 @@
         <v>2.18</v>
       </c>
       <c r="E641" t="n">
-        <v>0.8788320746194096</v>
+        <v>1.105934208623619</v>
       </c>
       <c r="F641" t="n">
         <v>0.00218</v>
@@ -15199,7 +15199,7 @@
         <v>1.82</v>
       </c>
       <c r="E642" t="n">
-        <v>0.8716289855507343</v>
+        <v>1.097936577124863</v>
       </c>
       <c r="F642" t="n">
         <v>0.00182</v>
@@ -15222,7 +15222,7 @@
         <v>2.17</v>
       </c>
       <c r="E643" t="n">
-        <v>0.874170293289442</v>
+        <v>1.100773698799137</v>
       </c>
       <c r="F643" t="n">
         <v>0.00217</v>
@@ -15245,7 +15245,7 @@
         <v>2.22</v>
       </c>
       <c r="E644" t="n">
-        <v>0.8727683031459544</v>
+        <v>1.099224558292559</v>
       </c>
       <c r="F644" t="n">
         <v>0.00222</v>
@@ -15268,7 +15268,7 @@
         <v>2.39</v>
       </c>
       <c r="E645" t="n">
-        <v>0.8728677829026457</v>
+        <v>1.099345605516858</v>
       </c>
       <c r="F645" t="n">
         <v>0.00239</v>
@@ -15291,7 +15291,7 @@
         <v>2.32</v>
       </c>
       <c r="E646" t="n">
-        <v>0.8729763091166484</v>
+        <v>1.099476351102511</v>
       </c>
       <c r="F646" t="n">
         <v>0.00232</v>
@@ -15314,7 +15314,7 @@
         <v>1.88</v>
       </c>
       <c r="E647" t="n">
-        <v>0.8755094298016347</v>
+        <v>1.102298417045833</v>
       </c>
       <c r="F647" t="n">
         <v>0.00188</v>
@@ -15337,7 +15337,7 @@
         <v>2.11</v>
       </c>
       <c r="E648" t="n">
-        <v>0.8712040857439572</v>
+        <v>1.097519756181148</v>
       </c>
       <c r="F648" t="n">
         <v>0.00211</v>
@@ -15360,7 +15360,7 @@
         <v>2.54</v>
       </c>
       <c r="E649" t="n">
-        <v>0.8752831926210625</v>
+        <v>1.102067322056933</v>
       </c>
       <c r="F649" t="n">
         <v>0.00254</v>
@@ -15383,7 +15383,7 @@
         <v>2.08</v>
       </c>
       <c r="E650" t="n">
-        <v>0.8744597980680742</v>
+        <v>1.101162163619932</v>
       </c>
       <c r="F650" t="n">
         <v>0.00208</v>
@@ -15406,7 +15406,7 @@
         <v>1.82</v>
       </c>
       <c r="E651" t="n">
-        <v>0.8737632128961803</v>
+        <v>1.100397477851567</v>
       </c>
       <c r="F651" t="n">
         <v>0.00182</v>
@@ -15429,7 +15429,7 @@
         <v>1.94</v>
       </c>
       <c r="E652" t="n">
-        <v>0.8693332598854269</v>
+        <v>1.09547774449736</v>
       </c>
       <c r="F652" t="n">
         <v>0.00194</v>
@@ -15452,7 +15452,7 @@
         <v>2.16</v>
       </c>
       <c r="E653" t="n">
-        <v>0.8716741903353697</v>
+        <v>1.098093719188546</v>
       </c>
       <c r="F653" t="n">
         <v>0.00216</v>
@@ -15475,7 +15475,7 @@
         <v>2.25</v>
       </c>
       <c r="E654" t="n">
-        <v>0.8692338687059625</v>
+        <v>1.095387346121843</v>
       </c>
       <c r="F654" t="n">
         <v>0.00225</v>
@@ -15498,7 +15498,7 @@
         <v>1.75</v>
       </c>
       <c r="E655" t="n">
-        <v>0.8679691076484215</v>
+        <v>1.093988896204953</v>
       </c>
       <c r="F655" t="n">
         <v>0.00175</v>
@@ -15521,7 +15521,7 @@
         <v>1.78</v>
       </c>
       <c r="E656" t="n">
-        <v>0.8656845268970816</v>
+        <v>1.091453479123582</v>
       </c>
       <c r="F656" t="n">
         <v>0.00178</v>
@@ -15544,7 +15544,7 @@
         <v>1.43</v>
       </c>
       <c r="E657" t="n">
-        <v>0.8692971173501248</v>
+        <v>1.095488187290246</v>
       </c>
       <c r="F657" t="n">
         <v>0.00143</v>
@@ -15567,7 +15567,7 @@
         <v>1.93</v>
       </c>
       <c r="E658" t="n">
-        <v>0.8683755939893082</v>
+        <v>1.094472040481999</v>
       </c>
       <c r="F658" t="n">
         <v>0.00193</v>
@@ -15590,7 +15590,7 @@
         <v>2.64</v>
       </c>
       <c r="E659" t="n">
-        <v>0.8716832313540878</v>
+        <v>1.098164753074326</v>
       </c>
       <c r="F659" t="n">
         <v>0.00264</v>
@@ -15613,7 +15613,7 @@
         <v>1.63</v>
       </c>
       <c r="E660" t="n">
-        <v>0.8647457926467644</v>
+        <v>1.09044745398416</v>
       </c>
       <c r="F660" t="n">
         <v>0.00163</v>
@@ -15636,7 +15636,7 @@
         <v>2</v>
       </c>
       <c r="E661" t="n">
-        <v>0.8677162038491987</v>
+        <v>1.093767910540504</v>
       </c>
       <c r="F661" t="n">
         <v>0.002</v>
@@ -15659,7 +15659,7 @@
         <v>2.3</v>
       </c>
       <c r="E662" t="n">
-        <v>0.8665963952547112</v>
+        <v>1.092540511857772</v>
       </c>
       <c r="F662" t="n">
         <v>0.0023</v>
@@ -15682,7 +15682,7 @@
         <v>1.79</v>
       </c>
       <c r="E663" t="n">
-        <v>0.8726145666069397</v>
+        <v>1.099252056602103</v>
       </c>
       <c r="F663" t="n">
         <v>0.00179</v>
@@ -15705,7 +15705,7 @@
         <v>1.62</v>
       </c>
       <c r="E664" t="n">
-        <v>0.8671923830219299</v>
+        <v>1.093224897685378</v>
       </c>
       <c r="F664" t="n">
         <v>0.00162</v>
@@ -15728,7 +15728,7 @@
         <v>1.58</v>
       </c>
       <c r="E665" t="n">
-        <v>0.8645111438474605</v>
+        <v>1.090256638374313</v>
       </c>
       <c r="F665" t="n">
         <v>0.00158</v>
@@ -15751,7 +15751,7 @@
         <v>1.93</v>
       </c>
       <c r="E666" t="n">
-        <v>0.8632929985910686</v>
+        <v>1.088918416028625</v>
       </c>
       <c r="F666" t="n">
         <v>0.00193</v>
@@ -15774,7 +15774,7 @@
         <v>2.45</v>
       </c>
       <c r="E667" t="n">
-        <v>0.8656484176193039</v>
+        <v>1.091549829226792</v>
       </c>
       <c r="F667" t="n">
         <v>0.00245</v>
@@ -15797,7 +15797,7 @@
         <v>1.93</v>
       </c>
       <c r="E668" t="n">
-        <v>0.8620301326831681</v>
+        <v>1.087550012818896</v>
       </c>
       <c r="F668" t="n">
         <v>0.00193</v>
@@ -15820,7 +15820,7 @@
         <v>2.02</v>
       </c>
       <c r="E669" t="n">
-        <v>0.8637441197993599</v>
+        <v>1.089482204364271</v>
       </c>
       <c r="F669" t="n">
         <v>0.00202</v>
@@ -15843,7 +15843,7 @@
         <v>1.68</v>
       </c>
       <c r="E670" t="n">
-        <v>0.8645652923362683</v>
+        <v>1.090418192037763</v>
       </c>
       <c r="F670" t="n">
         <v>0.00168</v>
@@ -15866,7 +15866,7 @@
         <v>2.31</v>
       </c>
       <c r="E671" t="n">
-        <v>0.8645201685441747</v>
+        <v>1.090383052059595</v>
       </c>
       <c r="F671" t="n">
         <v>0.00231</v>
@@ -15889,7 +15889,7 @@
         <v>1.97</v>
       </c>
       <c r="E672" t="n">
-        <v>0.8584241643006346</v>
+        <v>1.083590163379627</v>
       </c>
       <c r="F672" t="n">
         <v>0.00197</v>
@@ -15912,7 +15912,7 @@
         <v>2.14</v>
       </c>
       <c r="E673" t="n">
-        <v>0.8618948495220919</v>
+        <v>1.087474747881998</v>
       </c>
       <c r="F673" t="n">
         <v>0.00214</v>
@@ -15935,7 +15935,7 @@
         <v>2.07</v>
       </c>
       <c r="E674" t="n">
-        <v>0.8623277719196722</v>
+        <v>1.08796790167977</v>
       </c>
       <c r="F674" t="n">
         <v>0.00207</v>
@@ -15958,7 +15958,7 @@
         <v>2.05</v>
       </c>
       <c r="E675" t="n">
-        <v>0.8574421078995048</v>
+        <v>1.082523363754239</v>
       </c>
       <c r="F675" t="n">
         <v>0.00205</v>
@@ -15981,7 +15981,7 @@
         <v>2.26</v>
       </c>
       <c r="E676" t="n">
-        <v>0.8632208239685115</v>
+        <v>1.08898442843056</v>
       </c>
       <c r="F676" t="n">
         <v>0.00226</v>
@@ -16004,7 +16004,7 @@
         <v>1.51</v>
       </c>
       <c r="E677" t="n">
-        <v>0.8565323468542356</v>
+        <v>1.081526981425005</v>
       </c>
       <c r="F677" t="n">
         <v>0.00151</v>
@@ -16027,7 +16027,7 @@
         <v>1.8</v>
       </c>
       <c r="E678" t="n">
-        <v>0.8567845368479351</v>
+        <v>1.081818814365636</v>
       </c>
       <c r="F678" t="n">
         <v>0.0018</v>
@@ -16050,7 +16050,7 @@
         <v>1.41</v>
       </c>
       <c r="E679" t="n">
-        <v>0.8567935439312029</v>
+        <v>1.081839634307386</v>
       </c>
       <c r="F679" t="n">
         <v>0.00141</v>
@@ -16073,7 +16073,7 @@
         <v>1.84</v>
       </c>
       <c r="E680" t="n">
-        <v>0.8630223505421661</v>
+        <v>1.08880361377386</v>
       </c>
       <c r="F680" t="n">
         <v>0.00184</v>
@@ -16096,7 +16096,7 @@
         <v>1.61</v>
       </c>
       <c r="E681" t="n">
-        <v>0.8569646824153275</v>
+        <v>1.082050219687708</v>
       </c>
       <c r="F681" t="n">
         <v>0.00161</v>
@@ -16119,7 +16119,7 @@
         <v>1.58</v>
       </c>
       <c r="E682" t="n">
-        <v>0.8643396785177846</v>
+        <v>1.090293065094956</v>
       </c>
       <c r="F682" t="n">
         <v>0.00158</v>
@@ -16142,7 +16142,7 @@
         <v>1.47</v>
       </c>
       <c r="E683" t="n">
-        <v>0.853570320206315</v>
+        <v>1.078277894885521</v>
       </c>
       <c r="F683" t="n">
         <v>0.00147</v>
@@ -16165,7 +16165,7 @@
         <v>1.87</v>
       </c>
       <c r="E684" t="n">
-        <v>0.8579015717982155</v>
+        <v>1.083129587907153</v>
       </c>
       <c r="F684" t="n">
         <v>0.00187</v>
@@ -16188,7 +16188,7 @@
         <v>1.54</v>
       </c>
       <c r="E685" t="n">
-        <v>0.8526344578476126</v>
+        <v>1.077251697406236</v>
       </c>
       <c r="F685" t="n">
         <v>0.00154</v>
@@ -16211,7 +16211,7 @@
         <v>1.43</v>
       </c>
       <c r="E686" t="n">
-        <v>0.856172103363095</v>
+        <v>1.081217219101492</v>
       </c>
       <c r="F686" t="n">
         <v>0.00143</v>
@@ -16234,7 +16234,7 @@
         <v>1.88</v>
       </c>
       <c r="E687" t="n">
-        <v>0.8565683730104577</v>
+        <v>1.08167011405536</v>
       </c>
       <c r="F687" t="n">
         <v>0.00188</v>
@@ -16257,7 +16257,7 @@
         <v>1.46</v>
       </c>
       <c r="E688" t="n">
-        <v>0.8522115928684151</v>
+        <v>1.076808624945142</v>
       </c>
       <c r="F688" t="n">
         <v>0.00146</v>
@@ -16280,7 +16280,7 @@
         <v>2.52</v>
       </c>
       <c r="E689" t="n">
-        <v>0.8495315035411241</v>
+        <v>1.073819178386745</v>
       </c>
       <c r="F689" t="n">
         <v>0.00252</v>
@@ -16303,7 +16303,7 @@
         <v>1.93</v>
       </c>
       <c r="E690" t="n">
-        <v>0.8545874222865333</v>
+        <v>1.079485854786391</v>
       </c>
       <c r="F690" t="n">
         <v>0.00193</v>
@@ -16326,7 +16326,7 @@
         <v>1.43</v>
       </c>
       <c r="E691" t="n">
-        <v>0.8547134531818487</v>
+        <v>1.07963678759423</v>
       </c>
       <c r="F691" t="n">
         <v>0.00143</v>
@@ -16349,7 +16349,7 @@
         <v>1.61</v>
       </c>
       <c r="E692" t="n">
-        <v>0.8529223918555494</v>
+        <v>1.077643590768282</v>
       </c>
       <c r="F692" t="n">
         <v>0.00161</v>
@@ -16372,7 +16372,7 @@
         <v>2.16</v>
       </c>
       <c r="E693" t="n">
-        <v>0.8475271246969619</v>
+        <v>1.0716145633899</v>
       </c>
       <c r="F693" t="n">
         <v>0.00216</v>
@@ -16395,7 +16395,7 @@
         <v>2.97</v>
       </c>
       <c r="E694" t="n">
-        <v>0.8487404161072259</v>
+        <v>1.072983172159353</v>
       </c>
       <c r="F694" t="n">
         <v>0.00297</v>
@@ -16418,7 +16418,7 @@
         <v>1.73</v>
       </c>
       <c r="E695" t="n">
-        <v>0.8527874201729587</v>
+        <v>1.077522707161326</v>
       </c>
       <c r="F695" t="n">
         <v>0.00173</v>
@@ -16441,7 +16441,7 @@
         <v>1.95</v>
       </c>
       <c r="E696" t="n">
-        <v>0.8518247561009777</v>
+        <v>1.076455629075226</v>
       </c>
       <c r="F696" t="n">
         <v>0.00195</v>
@@ -16464,7 +16464,7 @@
         <v>1.79</v>
       </c>
       <c r="E697" t="n">
-        <v>0.8488123265849646</v>
+        <v>1.073093488510109</v>
       </c>
       <c r="F697" t="n">
         <v>0.00179</v>
@@ -16487,7 +16487,7 @@
         <v>1.66</v>
       </c>
       <c r="E698" t="n">
-        <v>0.8523195540860372</v>
+        <v>1.077029186107681</v>
       </c>
       <c r="F698" t="n">
         <v>0.00166</v>
@@ -16510,7 +16510,7 @@
         <v>2.02</v>
       </c>
       <c r="E699" t="n">
-        <v>0.8501249233336683</v>
+        <v>1.074583009252024</v>
       </c>
       <c r="F699" t="n">
         <v>0.00202</v>
@@ -16533,7 +16533,7 @@
         <v>1.76</v>
       </c>
       <c r="E700" t="n">
-        <v>0.8474462518874477</v>
+        <v>1.071593209209692</v>
       </c>
       <c r="F700" t="n">
         <v>0.00176</v>
@@ -16556,7 +16556,7 @@
         <v>1.74</v>
       </c>
       <c r="E701" t="n">
-        <v>0.8495404940835861</v>
+        <v>1.07394858510542</v>
       </c>
       <c r="F701" t="n">
         <v>0.00174</v>
@@ -16579,7 +16579,7 @@
         <v>1.76</v>
       </c>
       <c r="E702" t="n">
-        <v>0.8499540812059315</v>
+        <v>1.074421579803598</v>
       </c>
       <c r="F702" t="n">
         <v>0.00176</v>
@@ -16602,7 +16602,7 @@
         <v>1.86</v>
       </c>
       <c r="E703" t="n">
-        <v>0.8431085127332788</v>
+        <v>1.066760822563187</v>
       </c>
       <c r="F703" t="n">
         <v>0.00186</v>
@@ -16625,7 +16625,7 @@
         <v>1.74</v>
       </c>
       <c r="E704" t="n">
-        <v>0.8498551759896784</v>
+        <v>1.074330732445841</v>
       </c>
       <c r="F704" t="n">
         <v>0.00174</v>
@@ -16648,7 +16648,7 @@
         <v>1.77</v>
       </c>
       <c r="E705" t="n">
-        <v>0.8498192110717586</v>
+        <v>1.074300407450455</v>
       </c>
       <c r="F705" t="n">
         <v>0.00177</v>
@@ -16671,7 +16671,7 @@
         <v>1.89</v>
       </c>
       <c r="E706" t="n">
-        <v>0.8477877261561705</v>
+        <v>1.072035267425443</v>
       </c>
       <c r="F706" t="n">
         <v>0.00189</v>
@@ -16694,7 +16694,7 @@
         <v>1.83</v>
       </c>
       <c r="E707" t="n">
-        <v>0.8456764518430729</v>
+        <v>1.069679491767509</v>
       </c>
       <c r="F707" t="n">
         <v>0.00183</v>
@@ -16717,7 +16717,7 @@
         <v>1.85</v>
       </c>
       <c r="E708" t="n">
-        <v>0.8449489982932296</v>
+        <v>1.068883909079418</v>
       </c>
       <c r="F708" t="n">
         <v>0.00185</v>
@@ -16740,7 +16740,7 @@
         <v>1.68</v>
       </c>
       <c r="E709" t="n">
-        <v>0.8491359399745889</v>
+        <v>1.073585137601198</v>
       </c>
       <c r="F709" t="n">
         <v>0.00168</v>
@@ -16763,7 +16763,7 @@
         <v>1.22</v>
       </c>
       <c r="E710" t="n">
-        <v>0.8468891732052746</v>
+        <v>1.071078101801851</v>
       </c>
       <c r="F710" t="n">
         <v>0.00122</v>
@@ -16786,7 +16786,7 @@
         <v>1.47</v>
       </c>
       <c r="E711" t="n">
-        <v>0.8465747280976829</v>
+        <v>1.070735860087286</v>
       </c>
       <c r="F711" t="n">
         <v>0.00147</v>
@@ -16809,7 +16809,7 @@
         <v>1.53</v>
       </c>
       <c r="E712" t="n">
-        <v>0.8436022170435709</v>
+        <v>1.067413463633953</v>
       </c>
       <c r="F712" t="n">
         <v>0.00153</v>
@@ -16832,7 +16832,7 @@
         <v>2.4</v>
       </c>
       <c r="E713" t="n">
-        <v>0.8450028791311508</v>
+        <v>1.068994085441419</v>
       </c>
       <c r="F713" t="n">
         <v>0.0024</v>
@@ -16855,7 +16855,7 @@
         <v>1.54</v>
       </c>
       <c r="E714" t="n">
-        <v>0.8477248207771821</v>
+        <v>1.072054327620281</v>
       </c>
       <c r="F714" t="n">
         <v>0.00154</v>
@@ -16878,7 +16878,7 @@
         <v>1.42</v>
       </c>
       <c r="E715" t="n">
-        <v>0.8465747280976829</v>
+        <v>1.0707756037262</v>
       </c>
       <c r="F715" t="n">
         <v>0.00142</v>
@@ -16901,7 +16901,7 @@
         <v>1.28</v>
       </c>
       <c r="E716" t="n">
-        <v>0.8447963399246512</v>
+        <v>1.068792107023328</v>
       </c>
       <c r="F716" t="n">
         <v>0.00128</v>
@@ -16924,7 +16924,7 @@
         <v>1.93</v>
       </c>
       <c r="E717" t="n">
-        <v>0.8462333589793439</v>
+        <v>1.070412894528374</v>
       </c>
       <c r="F717" t="n">
         <v>0.00193</v>
@@ -16970,7 +16970,7 @@
         <v>1.831338308450954</v>
       </c>
       <c r="E719" t="n">
-        <v>0.8448053196647782</v>
+        <v>1.068822187720591</v>
       </c>
       <c r="F719" t="n">
         <v>0.00183</v>
@@ -16993,7 +16993,7 @@
         <v>2.241093483101497</v>
       </c>
       <c r="E720" t="n">
-        <v>0.8406498906586642</v>
+        <v>1.064169329702628</v>
       </c>
       <c r="F720" t="n">
         <v>0.00224</v>
@@ -17039,7 +17039,7 @@
         <v>1.301883251294063</v>
       </c>
       <c r="E722" t="n">
-        <v>0.8447694008271994</v>
+        <v>1.068799448629183</v>
       </c>
       <c r="F722" t="n">
         <v>0.0013</v>
@@ -17085,7 +17085,7 @@
         <v>1.541590088188167</v>
       </c>
       <c r="E724" t="n">
-        <v>0.8424982003291482</v>
+        <v>1.066271630015455</v>
       </c>
       <c r="F724" t="n">
         <v>0.00154</v>
@@ -17108,7 +17108,7 @@
         <v>1.681457700925004</v>
       </c>
       <c r="E725" t="n">
-        <v>0.8390086743169445</v>
+        <v>1.062359959248159</v>
       </c>
       <c r="F725" t="n">
         <v>0.00168</v>
@@ -17154,7 +17154,7 @@
         <v>1.541590088188167</v>
       </c>
       <c r="E727" t="n">
-        <v>0.8428392455871926</v>
+        <v>1.066674024333947</v>
       </c>
       <c r="F727" t="n">
         <v>0.00154</v>
@@ -17200,7 +17200,7 @@
         <v>1.431712261594487</v>
       </c>
       <c r="E729" t="n">
-        <v>0.8401655260202419</v>
+        <v>1.063688396849775</v>
       </c>
       <c r="F729" t="n">
         <v>0.00143</v>
@@ -17269,7 +17269,7 @@
         <v>1.351813596617522</v>
       </c>
       <c r="E732" t="n">
-        <v>0.8441408742315718</v>
+        <v>1.068153789851743</v>
       </c>
       <c r="F732" t="n">
         <v>0.00135</v>
@@ -17315,7 +17315,7 @@
         <v>1.511621645783098</v>
       </c>
       <c r="E734" t="n">
-        <v>0.8533543322683854</v>
+        <v>1.078484269826757</v>
       </c>
       <c r="F734" t="n">
         <v>0.00151</v>
@@ -17361,7 +17361,7 @@
         <v>1.841331040307527</v>
       </c>
       <c r="E736" t="n">
-        <v>0.8412419729505124</v>
+        <v>1.064921345810348</v>
       </c>
       <c r="F736" t="n">
         <v>0.00184</v>
@@ -17407,7 +17407,7 @@
         <v>1.711432148815722</v>
       </c>
       <c r="E738" t="n">
-        <v>0.8388114157723978</v>
+        <v>1.062202695461584</v>
       </c>
       <c r="F738" t="n">
         <v>0.00171</v>
@@ -17430,7 +17430,7 @@
         <v>1.671466422037846</v>
       </c>
       <c r="E739" t="n">
-        <v>0.8465118420890358</v>
+        <v>1.070851864696557</v>
       </c>
       <c r="F739" t="n">
         <v>0.00167</v>
@@ -17453,7 +17453,7 @@
         <v>2.231098384204516</v>
       </c>
       <c r="E740" t="n">
-        <v>0.842220001099803</v>
+        <v>1.066048536593386</v>
       </c>
       <c r="F740" t="n">
         <v>0.00223</v>
@@ -17499,7 +17499,7 @@
         <v>1.711432148815722</v>
       </c>
       <c r="E742" t="n">
-        <v>0.8404525497114955</v>
+        <v>1.064077242461156</v>
       </c>
       <c r="F742" t="n">
         <v>0.00171</v>
@@ -17522,7 +17522,7 @@
         <v>1.621511640414586</v>
       </c>
       <c r="E743" t="n">
-        <v>0.8439343802600155</v>
+        <v>1.067994055656253</v>
       </c>
       <c r="F743" t="n">
         <v>0.00162</v>
@@ -17545,7 +17545,7 @@
         <v>1.431712261594487</v>
       </c>
       <c r="E744" t="n">
-        <v>0.8377266708103103</v>
+        <v>1.06103585510357</v>
       </c>
       <c r="F744" t="n">
         <v>0.00143</v>
@@ -17591,7 +17591,7 @@
         <v>1.691449082887215</v>
       </c>
       <c r="E746" t="n">
-        <v>0.8400848043837292</v>
+        <v>1.063694010355448</v>
       </c>
       <c r="F746" t="n">
         <v>0.00169</v>
@@ -17660,7 +17660,7 @@
         <v>1.58154987275141</v>
       </c>
       <c r="E749" t="n">
-        <v>0.8441857656593591</v>
+        <v>1.068310695434536</v>
       </c>
       <c r="F749" t="n">
         <v>0.00158</v>
@@ -17706,7 +17706,7 @@
         <v>1.881302740124513</v>
       </c>
       <c r="E751" t="n">
-        <v>0.8380493735426947</v>
+        <v>1.06143283031967</v>
       </c>
       <c r="F751" t="n">
         <v>0.00188</v>
@@ -17752,7 +17752,7 @@
         <v>1.841331040307527</v>
       </c>
       <c r="E753" t="n">
-        <v>0.8415918816786622</v>
+        <v>1.065420307991541</v>
       </c>
       <c r="F753" t="n">
         <v>0.00184</v>
@@ -17775,7 +17775,7 @@
         <v>1.441700384962146</v>
       </c>
       <c r="E754" t="n">
-        <v>0.8378431992937787</v>
+        <v>1.061220918419736</v>
       </c>
       <c r="F754" t="n">
         <v>0.00144</v>
@@ -17821,7 +17821,7 @@
         <v>1.661475248085267</v>
       </c>
       <c r="E756" t="n">
-        <v>0.8391073073035343</v>
+        <v>1.062650654477182</v>
       </c>
       <c r="F756" t="n">
         <v>0.00166</v>
@@ -17867,7 +17867,7 @@
         <v>1.761391495380854</v>
       </c>
       <c r="E758" t="n">
-        <v>0.840291096305953</v>
+        <v>1.063989784950511</v>
       </c>
       <c r="F758" t="n">
         <v>0.00176</v>
@@ -17890,7 +17890,7 @@
         <v>1.691449082887215</v>
       </c>
       <c r="E759" t="n">
-        <v>0.838130053369035</v>
+        <v>1.061572711326671</v>
       </c>
       <c r="F759" t="n">
         <v>0.00169</v>
@@ -17936,7 +17936,7 @@
         <v>1.541590088188167</v>
       </c>
       <c r="E761" t="n">
-        <v>0.8407037126365599</v>
+        <v>1.064472768334741</v>
       </c>
       <c r="F761" t="n">
         <v>0.00154</v>
@@ -17982,7 +17982,7 @@
         <v>1.761391495380854</v>
       </c>
       <c r="E763" t="n">
-        <v>0.8405332789014246</v>
+        <v>1.064291279400066</v>
       </c>
       <c r="F763" t="n">
         <v>0.00176</v>
@@ -18005,7 +18005,7 @@
         <v>1.651484180971771</v>
       </c>
       <c r="E764" t="n">
-        <v>0.8380314449174665</v>
+        <v>1.061491431413804</v>
       </c>
       <c r="F764" t="n">
         <v>0.00165</v>
@@ -18051,7 +18051,7 @@
         <v>1.771383639983163</v>
       </c>
       <c r="E766" t="n">
-        <v>0.8363465195341951</v>
+        <v>1.059607964457749</v>
       </c>
       <c r="F766" t="n">
         <v>0.00177</v>
@@ -18097,7 +18097,7 @@
         <v>1.661475248085267</v>
       </c>
       <c r="E768" t="n">
-        <v>0.8355222450416631</v>
+        <v>1.058691257897557</v>
       </c>
       <c r="F768" t="n">
         <v>0.00166</v>
@@ -18120,7 +18120,7 @@
         <v>1.951256005756292</v>
       </c>
       <c r="E769" t="n">
-        <v>0.8349310243190592</v>
+        <v>1.058031481591969</v>
       </c>
       <c r="F769" t="n">
         <v>0.00195</v>
@@ -18166,7 +18166,7 @@
         <v>1.761391495380854</v>
       </c>
       <c r="E771" t="n">
-        <v>0.838076266633993</v>
+        <v>1.061571079880766</v>
       </c>
       <c r="F771" t="n">
         <v>0.00176</v>
@@ -18189,7 +18189,7 @@
         <v>1.361800279042415</v>
       </c>
       <c r="E772" t="n">
-        <v>0.834904152766311</v>
+        <v>1.058015955298693</v>
       </c>
       <c r="F772" t="n">
         <v>0.00136</v>
@@ -18235,7 +18235,7 @@
         <v>1.611521020650988</v>
       </c>
       <c r="E774" t="n">
-        <v>0.8329072158813121</v>
+        <v>1.055779898841693</v>
       </c>
       <c r="F774" t="n">
         <v>0.00161</v>
@@ -18281,7 +18281,7 @@
         <v>1.681457700925004</v>
       </c>
       <c r="E776" t="n">
-        <v>0.8348951956229578</v>
+        <v>1.058025640898138</v>
       </c>
       <c r="F776" t="n">
         <v>0.00168</v>
@@ -18327,7 +18327,7 @@
         <v>1.851323850653904</v>
       </c>
       <c r="E778" t="n">
-        <v>0.832558080237221</v>
+        <v>1.055406660592199</v>
       </c>
       <c r="F778" t="n">
         <v>0.00185</v>
@@ -18350,7 +18350,7 @@
         <v>1.651484180971771</v>
       </c>
       <c r="E779" t="n">
-        <v>0.8341876459107064</v>
+        <v>1.057249411975014</v>
       </c>
       <c r="F779" t="n">
         <v>0.00165</v>
@@ -18396,7 +18396,7 @@
         <v>1.921275617916388</v>
       </c>
       <c r="E781" t="n">
-        <v>0.8356835025170833</v>
+        <v>1.058941125814596</v>
       </c>
       <c r="F781" t="n">
         <v>0.00192</v>
@@ -18419,7 +18419,7 @@
         <v>1.671466422037846</v>
       </c>
       <c r="E782" t="n">
-        <v>0.8305444430932507</v>
+        <v>1.053169866816276</v>
       </c>
       <c r="F782" t="n">
         <v>0.00167</v>
@@ -18465,7 +18465,7 @@
         <v>1.941262475813098</v>
       </c>
       <c r="E784" t="n">
-        <v>0.8354147437391589</v>
+        <v>1.058658051317745</v>
       </c>
       <c r="F784" t="n">
         <v>0.00194</v>
@@ -18488,7 +18488,7 @@
         <v>1.76</v>
       </c>
       <c r="E785" t="n">
-        <v>0.8330056956582221</v>
+        <v>1.055959108027635</v>
       </c>
       <c r="F785" t="n">
         <v>0.00176</v>
@@ -18511,7 +18511,7 @@
         <v>1.82</v>
       </c>
       <c r="E786" t="n">
-        <v>0.8389548755497794</v>
+        <v>1.062656588893791</v>
       </c>
       <c r="F786" t="n">
         <v>0.00182</v>
@@ -18534,7 +18534,7 @@
         <v>1.6</v>
       </c>
       <c r="E787" t="n">
-        <v>0.8308576075965689</v>
+        <v>1.053561448457446</v>
       </c>
       <c r="F787" t="n">
         <v>0.0016</v>
@@ -18557,7 +18557,7 @@
         <v>1.85</v>
       </c>
       <c r="E788" t="n">
-        <v>0.8354684940223054</v>
+        <v>1.05875830356536</v>
       </c>
       <c r="F788" t="n">
         <v>0.00185</v>
@@ -18580,7 +18580,7 @@
         <v>1.62</v>
       </c>
       <c r="E789" t="n">
-        <v>0.83540578543021</v>
+        <v>1.058697623555795</v>
       </c>
       <c r="F789" t="n">
         <v>0.00162</v>
@@ -18603,7 +18603,7 @@
         <v>1.33</v>
       </c>
       <c r="E790" t="n">
-        <v>0.8307860249321114</v>
+        <v>1.053510200464635</v>
       </c>
       <c r="F790" t="n">
         <v>0.00133</v>
@@ -18626,7 +18626,7 @@
         <v>1.66</v>
       </c>
       <c r="E791" t="n">
-        <v>0.8287106963948605</v>
+        <v>1.05118320792601</v>
       </c>
       <c r="F791" t="n">
         <v>0.00166</v>
@@ -18649,7 +18649,7 @@
         <v>1.46</v>
       </c>
       <c r="E792" t="n">
-        <v>0.8318330516896738</v>
+        <v>1.0547082198576</v>
       </c>
       <c r="F792" t="n">
         <v>0.00146</v>
@@ -18672,7 +18672,7 @@
         <v>1.77</v>
       </c>
       <c r="E793" t="n">
-        <v>0.8307233911733554</v>
+        <v>1.053469021266814</v>
       </c>
       <c r="F793" t="n">
         <v>0.00177</v>
@@ -18695,7 +18695,7 @@
         <v>1.35</v>
       </c>
       <c r="E794" t="n">
-        <v>0.8293278128585159</v>
+        <v>1.051907477722593</v>
       </c>
       <c r="F794" t="n">
         <v>0.00135</v>
@@ -18718,7 +18718,7 @@
         <v>2.02</v>
       </c>
       <c r="E795" t="n">
-        <v>0.8292294254576172</v>
+        <v>1.05181637401577</v>
       </c>
       <c r="F795" t="n">
         <v>0.00202</v>
@@ -18741,7 +18741,7 @@
         <v>1.7</v>
       </c>
       <c r="E796" t="n">
-        <v>0.828961108743663</v>
+        <v>1.051523774775527</v>
       </c>
       <c r="F796" t="n">
         <v>0.0017</v>
@@ -18764,7 +18764,7 @@
         <v>1.7</v>
       </c>
       <c r="E797" t="n">
-        <v>0.8296677156234106</v>
+        <v>1.052328945162651</v>
       </c>
       <c r="F797" t="n">
         <v>0.0017</v>
@@ -18787,7 +18787,7 @@
         <v>1.51</v>
       </c>
       <c r="E798" t="n">
-        <v>0.830571284784286</v>
+        <v>1.053356434466668</v>
       </c>
       <c r="F798" t="n">
         <v>0.00151</v>
@@ -18810,7 +18810,7 @@
         <v>1.91</v>
       </c>
       <c r="E799" t="n">
-        <v>0.8287732979809485</v>
+        <v>1.051341337821634</v>
       </c>
       <c r="F799" t="n">
         <v>0.00191</v>
@@ -18833,7 +18833,7 @@
         <v>1.64</v>
       </c>
       <c r="E800" t="n">
-        <v>0.8276376819595338</v>
+        <v>1.050071969840582</v>
       </c>
       <c r="F800" t="n">
         <v>0.00164</v>
@@ -18856,7 +18856,7 @@
         <v>1.84</v>
       </c>
       <c r="E801" t="n">
-        <v>0.8298018958869758</v>
+        <v>1.052519453923226</v>
       </c>
       <c r="F801" t="n">
         <v>0.00184</v>
@@ -18879,7 +18879,7 @@
         <v>1.45</v>
       </c>
       <c r="E802" t="n">
-        <v>0.8294083134793514</v>
+        <v>1.05208599107938</v>
       </c>
       <c r="F802" t="n">
         <v>0.00145</v>
@@ -18902,7 +18902,7 @@
         <v>1.87</v>
       </c>
       <c r="E803" t="n">
-        <v>0.8274409945419696</v>
+        <v>1.049879585335931</v>
       </c>
       <c r="F803" t="n">
         <v>0.00187</v>
@@ -18925,7 +18925,7 @@
         <v>1.2</v>
       </c>
       <c r="E804" t="n">
-        <v>0.8254210504603346</v>
+        <v>1.047612697034974</v>
       </c>
       <c r="F804" t="n">
         <v>0.0012</v>
@@ -18948,7 +18948,7 @@
         <v>1.81</v>
       </c>
       <c r="E805" t="n">
-        <v>0.827700266392129</v>
+        <v>1.05019120662038</v>
       </c>
       <c r="F805" t="n">
         <v>0.00181</v>
@@ -18971,7 +18971,7 @@
         <v>1.47</v>
       </c>
       <c r="E806" t="n">
-        <v>0.8274141742961567</v>
+        <v>1.049878591000924</v>
       </c>
       <c r="F806" t="n">
         <v>0.00147</v>
@@ -18994,7 +18994,7 @@
         <v>2.17</v>
       </c>
       <c r="E807" t="n">
-        <v>0.8286123244957251</v>
+        <v>1.051238231392732</v>
       </c>
       <c r="F807" t="n">
         <v>0.00217</v>
@@ -19017,7 +19017,7 @@
         <v>1.68</v>
       </c>
       <c r="E808" t="n">
-        <v>0.8249296288789429</v>
+        <v>1.047098382100717</v>
       </c>
       <c r="F808" t="n">
         <v>0.00168</v>
@@ -19040,7 +19040,7 @@
         <v>1.7</v>
       </c>
       <c r="E809" t="n">
-        <v>0.8235539768499502</v>
+        <v>1.045555999947524</v>
       </c>
       <c r="F809" t="n">
         <v>0.0017</v>
@@ -19063,7 +19063,7 @@
         <v>1.74</v>
       </c>
       <c r="E810" t="n">
-        <v>0.8275125160958531</v>
+        <v>1.05002837607907</v>
       </c>
       <c r="F810" t="n">
         <v>0.00174</v>
@@ -19086,7 +19086,7 @@
         <v>1.48</v>
       </c>
       <c r="E811" t="n">
-        <v>0.8290594894044307</v>
+        <v>1.05178096335801</v>
       </c>
       <c r="F811" t="n">
         <v>0.00148</v>
@@ -19109,7 +19109,7 @@
         <v>1.51</v>
       </c>
       <c r="E812" t="n">
-        <v>0.8291578725365382</v>
+        <v>1.051901540916865</v>
       </c>
       <c r="F812" t="n">
         <v>0.00151</v>
@@ -19132,7 +19132,7 @@
         <v>2.08</v>
       </c>
       <c r="E813" t="n">
-        <v>0.8241792132371292</v>
+        <v>1.046299845645536</v>
       </c>
       <c r="F813" t="n">
         <v>0.00208</v>
@@ -19155,7 +19155,7 @@
         <v>1.78</v>
       </c>
       <c r="E814" t="n">
-        <v>0.8294262027308857</v>
+        <v>1.052223298646312</v>
       </c>
       <c r="F814" t="n">
         <v>0.00178</v>
@@ -19178,7 +19178,7 @@
         <v>1.54</v>
       </c>
       <c r="E815" t="n">
-        <v>0.8221788086730908</v>
+        <v>1.044062550072746</v>
       </c>
       <c r="F815" t="n">
         <v>0.00154</v>
@@ -19201,7 +19201,7 @@
         <v>1.41</v>
       </c>
       <c r="E816" t="n">
-        <v>0.8207238004717003</v>
+        <v>1.042430060890222</v>
       </c>
       <c r="F816" t="n">
         <v>0.00141</v>
@@ -19224,7 +19224,7 @@
         <v>1.49</v>
       </c>
       <c r="E817" t="n">
-        <v>0.8261895788600324</v>
+        <v>1.048605512654048</v>
       </c>
       <c r="F817" t="n">
         <v>0.00149</v>
@@ -19247,7 +19247,7 @@
         <v>1.31</v>
       </c>
       <c r="E818" t="n">
-        <v>0.8242596080261498</v>
+        <v>1.046434210582191</v>
       </c>
       <c r="F818" t="n">
         <v>0.00131</v>
@@ -19270,7 +19270,7 @@
         <v>1.74</v>
       </c>
       <c r="E819" t="n">
-        <v>0.8243846698720305</v>
+        <v>1.046584970036571</v>
       </c>
       <c r="F819" t="n">
         <v>0.00174</v>
@@ -19293,7 +19293,7 @@
         <v>1.58</v>
       </c>
       <c r="E820" t="n">
-        <v>0.8223395176481738</v>
+        <v>1.044287498586378</v>
       </c>
       <c r="F820" t="n">
         <v>0.00158</v>
@@ -19316,7 +19316,7 @@
         <v>1.75</v>
       </c>
       <c r="E821" t="n">
-        <v>0.8253674378331838</v>
+        <v>1.047712657641208</v>
       </c>
       <c r="F821" t="n">
         <v>0.00175</v>
@@ -19339,7 +19339,7 @@
         <v>2.2</v>
       </c>
       <c r="E822" t="n">
-        <v>0.8238933784835376</v>
+        <v>1.046059968071654</v>
       </c>
       <c r="F822" t="n">
         <v>0.0022</v>
@@ -19362,7 +19362,7 @@
         <v>1.910942175995914</v>
       </c>
       <c r="E823" t="n">
-        <v>0.8267347893599111</v>
+        <v>1.049273614796683</v>
       </c>
       <c r="F823" t="n">
         <v>0.00191</v>
@@ -19408,7 +19408,7 @@
         <v>1.611117624507907</v>
       </c>
       <c r="E825" t="n">
-        <v>0.8231431616572088</v>
+        <v>1.045233010370215</v>
       </c>
       <c r="F825" t="n">
         <v>0.00161</v>
@@ -19431,7 +19431,7 @@
         <v>1.301383878799795</v>
       </c>
       <c r="E826" t="n">
-        <v>0.8229020511052816</v>
+        <v>1.044970644428595</v>
       </c>
       <c r="F826" t="n">
         <v>0.0013</v>
@@ -19477,7 +19477,7 @@
         <v>1.751028269332052</v>
       </c>
       <c r="E828" t="n">
-        <v>0.8238755145051631</v>
+        <v>1.046078554533426</v>
       </c>
       <c r="F828" t="n">
         <v>0.00175</v>
@@ -19523,7 +19523,7 @@
         <v>1.781010948871455</v>
       </c>
       <c r="E830" t="n">
-        <v>0.821955612726241</v>
+        <v>1.043921961893151</v>
       </c>
       <c r="F830" t="n">
         <v>0.00178</v>
@@ -19546,7 +19546,7 @@
         <v>1.591131672741134</v>
       </c>
       <c r="E831" t="n">
-        <v>0.827503575830155</v>
+        <v>1.0501886830084</v>
       </c>
       <c r="F831" t="n">
         <v>0.00159</v>
@@ -19615,7 +19615,7 @@
         <v>1.661083983427689</v>
       </c>
       <c r="E834" t="n">
-        <v>0.8181186371446638</v>
+        <v>1.039608656600227</v>
       </c>
       <c r="F834" t="n">
         <v>0.00166</v>
@@ -19661,7 +19661,7 @@
         <v>1.451240848377691</v>
       </c>
       <c r="E836" t="n">
-        <v>0.8215628188197039</v>
+        <v>1.043507601010769</v>
       </c>
       <c r="F836" t="n">
         <v>0.00145</v>
@@ -19707,7 +19707,7 @@
         <v>1.511191582824627</v>
       </c>
       <c r="E838" t="n">
-        <v>0.8203846739825466</v>
+        <v>1.042187217514766</v>
       </c>
       <c r="F838" t="n">
         <v>0.00151</v>
@@ -19753,7 +19753,7 @@
         <v>1.431258187749506</v>
       </c>
       <c r="E840" t="n">
-        <v>0.8203132826838503</v>
+        <v>1.042116252709246</v>
       </c>
       <c r="F840" t="n">
         <v>0.00143</v>
@@ -19822,7 +19822,7 @@
         <v>1.491207564358497</v>
       </c>
       <c r="E843" t="n">
-        <v>0.8187876056838215</v>
+        <v>1.040402858040278</v>
       </c>
       <c r="F843" t="n">
         <v>0.00149</v>
@@ -19868,7 +19868,7 @@
         <v>1.341342610968577</v>
       </c>
       <c r="E845" t="n">
-        <v>0.8188143668100453</v>
+        <v>1.040442714986497</v>
       </c>
       <c r="F845" t="n">
         <v>0.00134</v>
@@ -19914,7 +19914,7 @@
         <v>1.341342610968577</v>
       </c>
       <c r="E847" t="n">
-        <v>0.8174230314702221</v>
+        <v>1.038880419461076</v>
       </c>
       <c r="F847" t="n">
         <v>0.00134</v>
@@ -19983,7 +19983,7 @@
         <v>1.261427762497718</v>
       </c>
       <c r="E850" t="n">
-        <v>0.8170574423008761</v>
+        <v>1.038476904188804</v>
       </c>
       <c r="F850" t="n">
         <v>0.00126</v>
@@ -20006,7 +20006,7 @@
         <v>1.561153419750922</v>
       </c>
       <c r="E851" t="n">
-        <v>0.8233664254284053</v>
+        <v>1.045610712054806</v>
       </c>
       <c r="F851" t="n">
         <v>0.00156</v>
@@ -20098,7 +20098,7 @@
         <v>1.551160855617495</v>
       </c>
       <c r="E855" t="n">
-        <v>0.8221252404832768</v>
+        <v>1.044219924317158</v>
       </c>
       <c r="F855" t="n">
         <v>0.00155</v>
@@ -20167,7 +20167,7 @@
         <v>1.810994202089007</v>
       </c>
       <c r="E858" t="n">
-        <v>0.8185289242543529</v>
+        <v>1.04016848715441</v>
       </c>
       <c r="F858" t="n">
         <v>0.00181</v>
@@ -20213,7 +20213,7 @@
         <v>1.58113883008419</v>
       </c>
       <c r="E860" t="n">
-        <v>0.8171198575391788</v>
+        <v>1.038585816655981</v>
       </c>
       <c r="F860" t="n">
         <v>0.00158</v>
@@ -20282,7 +20282,7 @@
         <v>1.571146078504478</v>
       </c>
       <c r="E863" t="n">
-        <v>0.8174319487071376</v>
+        <v>1.038948321037893</v>
       </c>
       <c r="F863" t="n">
         <v>0.00157</v>
@@ -20328,7 +20328,7 @@
         <v>1.31137332594498</v>
       </c>
       <c r="E865" t="n">
-        <v>0.8183951302409253</v>
+        <v>1.040046115123437</v>
       </c>
       <c r="F865" t="n">
         <v>0.00131</v>
@@ -20374,7 +20374,7 @@
         <v>1.561153419750922</v>
       </c>
       <c r="E867" t="n">
-        <v>0.8172090238972695</v>
+        <v>1.038715673167645</v>
       </c>
       <c r="F867" t="n">
         <v>0.00156</v>
@@ -20397,7 +20397,7 @@
         <v>1.431258187749506</v>
       </c>
       <c r="E868" t="n">
-        <v>0.8177351468868458</v>
+        <v>1.039315049009991</v>
       </c>
       <c r="F868" t="n">
         <v>0.00143</v>
@@ -20443,7 +20443,7 @@
         <v>1.461232356608626</v>
       </c>
       <c r="E870" t="n">
-        <v>0.8172179406451467</v>
+        <v>1.038740208489677</v>
       </c>
       <c r="F870" t="n">
         <v>0.00146</v>
@@ -20512,7 +20512,7 @@
         <v>1.271416532848303</v>
       </c>
       <c r="E873" t="n">
-        <v>0.8174230314702221</v>
+        <v>1.038981627937656</v>
       </c>
       <c r="F873" t="n">
         <v>0.00127</v>
@@ -20558,7 +20558,7 @@
         <v>1.791005304291419</v>
       </c>
       <c r="E875" t="n">
-        <v>0.8135815988942436</v>
+        <v>1.034647862289267</v>
       </c>
       <c r="F875" t="n">
         <v>0.00179</v>
@@ -20604,7 +20604,7 @@
         <v>1.810994202089007</v>
       </c>
       <c r="E877" t="n">
-        <v>0.8123880497057306</v>
+        <v>1.033307749217715</v>
       </c>
       <c r="F877" t="n">
         <v>0.00181</v>
@@ -20650,7 +20650,7 @@
         <v>1.491207564358497</v>
       </c>
       <c r="E879" t="n">
-        <v>0.8175032873360386</v>
+        <v>1.039101250813202</v>
       </c>
       <c r="F879" t="n">
         <v>0.00149</v>
@@ -20696,7 +20696,7 @@
         <v>1.860967490312499</v>
       </c>
       <c r="E881" t="n">
-        <v>0.8136706843883321</v>
+        <v>1.034777443151699</v>
       </c>
       <c r="F881" t="n">
         <v>0.00186</v>
@@ -20719,7 +20719,7 @@
         <v>1.591131672741134</v>
       </c>
       <c r="E882" t="n">
-        <v>0.8174765351973717</v>
+        <v>1.039090301694207</v>
       </c>
       <c r="F882" t="n">
         <v>0.00159</v>
@@ -20742,7 +20742,7 @@
         <v>1.431258187749506</v>
       </c>
       <c r="E883" t="n">
-        <v>0.8144725454673755</v>
+        <v>1.035703665410841</v>
       </c>
       <c r="F883" t="n">
         <v>0.00143</v>
@@ -20857,7 +20857,7 @@
         <v>1.501199520383616</v>
       </c>
       <c r="E888" t="n">
-        <v>0.815711299484948</v>
+        <v>1.037114127970639</v>
       </c>
       <c r="F888" t="n">
         <v>0.0015</v>
@@ -20903,7 +20903,7 @@
         <v>1.791005304291419</v>
       </c>
       <c r="E890" t="n">
-        <v>0.8145972942380679</v>
+        <v>1.035863981191282</v>
       </c>
       <c r="F890" t="n">
         <v>0.00179</v>
@@ -20949,7 +20949,7 @@
         <v>1.781010948871455</v>
       </c>
       <c r="E892" t="n">
-        <v>0.8106963303949002</v>
+        <v>1.031459316363294</v>
       </c>
       <c r="F892" t="n">
         <v>0.00178</v>
@@ -20972,7 +20972,7 @@
         <v>1.930932417253385</v>
       </c>
       <c r="E893" t="n">
-        <v>0.8130025928119442</v>
+        <v>1.034079352069204</v>
       </c>
       <c r="F893" t="n">
         <v>0.00193</v>
@@ -21018,7 +21018,7 @@
         <v>1.491207564358497</v>
       </c>
       <c r="E895" t="n">
-        <v>0.8105539033610561</v>
+        <v>1.031317203949679</v>
       </c>
       <c r="F895" t="n">
         <v>0.00149</v>
@@ -21064,7 +21064,7 @@
         <v>1.701058493997193</v>
       </c>
       <c r="E897" t="n">
-        <v>0.816460089814824</v>
+        <v>1.038008845016047</v>
       </c>
       <c r="F897" t="n">
         <v>0.0017</v>
@@ -21087,7 +21087,7 @@
         <v>1.461232356608626</v>
       </c>
       <c r="E898" t="n">
-        <v>0.8133232624756244</v>
+        <v>1.034470798602156</v>
       </c>
       <c r="F898" t="n">
         <v>0.00146</v>
@@ -21133,7 +21133,7 @@
         <v>1.611117624507907</v>
       </c>
       <c r="E900" t="n">
-        <v>0.8135905073520255</v>
+        <v>1.034782759624745</v>
       </c>
       <c r="F900" t="n">
         <v>0.00161</v>
@@ -21179,7 +21179,7 @@
         <v>1.910942175995914</v>
       </c>
       <c r="E902" t="n">
-        <v>0.8210272543935042</v>
+        <v>1.043193256856413</v>
       </c>
       <c r="F902" t="n">
         <v>0.00191</v>
@@ -21202,7 +21202,7 @@
         <v>1.771016657177453</v>
       </c>
       <c r="E903" t="n">
-        <v>0.8091299195131936</v>
+        <v>1.029742873381068</v>
       </c>
       <c r="F903" t="n">
         <v>0.00177</v>
@@ -21271,7 +21271,7 @@
         <v>1.511191582824627</v>
       </c>
       <c r="E906" t="n">
-        <v>0.8115242906760779</v>
+        <v>1.032464853845205</v>
       </c>
       <c r="F906" t="n">
         <v>0.00151</v>
@@ -21317,7 +21317,7 @@
         <v>2.080865204668481</v>
       </c>
       <c r="E908" t="n">
-        <v>0.8114352542428643</v>
+        <v>1.032375012842809</v>
       </c>
       <c r="F908" t="n">
         <v>0.00208</v>
@@ -21363,7 +21363,7 @@
         <v>1.391294361377203</v>
       </c>
       <c r="E910" t="n">
-        <v>0.8135014236904639</v>
+        <v>1.034722778141149</v>
       </c>
       <c r="F910" t="n">
         <v>0.00139</v>
@@ -21409,7 +21409,7 @@
         <v>1.830983342360056</v>
       </c>
       <c r="E912" t="n">
-        <v>0.8084981935146438</v>
+        <v>1.029067859984506</v>
       </c>
       <c r="F912" t="n">
         <v>0.00183</v>
@@ -21455,7 +21455,7 @@
         <v>1.511191582824627</v>
       </c>
       <c r="E914" t="n">
-        <v>0.8117736035170013</v>
+        <v>1.032786766378142</v>
       </c>
       <c r="F914" t="n">
         <v>0.00151</v>
@@ -21478,7 +21478,7 @@
         <v>1.820988742414406</v>
       </c>
       <c r="E915" t="n">
-        <v>0.8076975614467052</v>
+        <v>1.028175211942363</v>
       </c>
       <c r="F915" t="n">
         <v>0.00182</v>

</xml_diff>